<commit_message>
Changed stats a bit to better reflect contribution in their respective categories
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/CommitTable.xlsx
+++ b/meta/dudpy-planning/CommitTable.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F5A86E-861E-4F92-9A20-F2FEEC40FD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952BB5B-84F7-4CC6-B7A5-2CA97988AD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-405" yWindow="1695" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -4331,7 +4331,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Last 5</a:t>
+              <a:t>Last 6</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -4511,7 +4511,7 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4660,7 +4660,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Last 5</a:t>
+              <a:t>Last 14</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -4841,10 +4841,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>337</c:v>
+                  <c:v>816</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>465</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>316</c:v>
@@ -9396,8 +9396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P100" sqref="P100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16499,7 +16499,7 @@
         <v>182</v>
       </c>
       <c r="H202">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I202" s="17" cm="1">
         <f t="array" ref="I202">SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (ROW(I$3:I$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(I$3:I$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
@@ -16507,7 +16507,7 @@
       </c>
       <c r="J202" s="17" cm="1">
         <f t="array" ref="J202">SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (ROW(J$3:J$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(J$3:J$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="K202" s="17" cm="1">
         <f t="array" ref="K202">SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (ROW(K$3:K$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(K$3:K$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
@@ -16527,26 +16527,26 @@
         <v>182</v>
       </c>
       <c r="H203">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I203" cm="1">
-        <f t="array" ref="I203">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0) * (ROW(I$3:I$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0), ROW(I$3:I$200)), MIN($H$202, COUNTIFS($G$3:$G$200, "&lt;&gt;", I$3:I$200, "&gt;0")))))), 0)</f>
-        <v>337</v>
+        <f t="array" ref="I203">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0) * (ROW(I$3:I$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0), ROW(I$3:I$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", I$3:I$200, "&gt;0")))))), 0)</f>
+        <v>816</v>
       </c>
       <c r="J203" cm="1">
-        <f t="array" ref="J203">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0) * (ROW(J$3:J$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0), ROW(J$3:J$200)), MIN($H$202, COUNTIFS($G$3:$G$200, "&lt;&gt;", J$3:J$200, "&gt;0")))))), 0)</f>
-        <v>93</v>
+        <f t="array" ref="J203">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0) * (ROW(J$3:J$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0), ROW(J$3:J$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", J$3:J$200, "&gt;0")))))), 0)</f>
+        <v>465</v>
       </c>
       <c r="K203" cm="1">
-        <f t="array" ref="K203">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0) * (ROW(K$3:K$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0), ROW(K$3:K$200)), MIN($H$202, COUNTIFS($G$3:$G$200, "&lt;&gt;", K$3:K$200, "&gt;0")))))), 0)</f>
+        <f t="array" ref="K203">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0) * (ROW(K$3:K$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0), ROW(K$3:K$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", K$3:K$200, "&gt;0")))))), 0)</f>
         <v>316</v>
       </c>
       <c r="L203" cm="1">
-        <f t="array" ref="L203">IFERROR(SUM(_xlfn._xlws.FILTER(L$3:L$200, ($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0) * (ROW(L$3:L$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0), ROW(L$3:L$200)), MIN($H$202, COUNTIFS($G$3:$G$200, "&lt;&gt;", L$3:L$200, "&gt;0")))))), 0)</f>
+        <f t="array" ref="L203">IFERROR(SUM(_xlfn._xlws.FILTER(L$3:L$200, ($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0) * (ROW(L$3:L$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0), ROW(L$3:L$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", L$3:L$200, "&gt;0")))))), 0)</f>
         <v>574</v>
       </c>
       <c r="M203" cm="1">
-        <f t="array" ref="M203">IFERROR(SUM(_xlfn._xlws.FILTER(M$3:M$200, ($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0) * (ROW(M$3:M$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0), ROW(M$3:M$200)), MIN($H$202, COUNTIFS($G$3:$G$200, "&lt;&gt;", M$3:M$200, "&gt;0")))))), 0)</f>
+        <f t="array" ref="M203">IFERROR(SUM(_xlfn._xlws.FILTER(M$3:M$200, ($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0) * (ROW(M$3:M$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0), ROW(M$3:M$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", M$3:M$200, "&gt;0")))))), 0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Housekeeping and change to stats
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/CommitTable.xlsx
+++ b/meta/dudpy-planning/CommitTable.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952BB5B-84F7-4CC6-B7A5-2CA97988AD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09BE415-E6A6-4BC0-8B56-2BE01682522B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="1695" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="194">
   <si>
     <t>Datei</t>
   </si>
@@ -649,6 +649,30 @@
   </si>
   <si>
     <t>often a lot shorter than gui source code</t>
+  </si>
+  <si>
+    <t>Json Design = Hard</t>
+  </si>
+  <si>
+    <t>bridge format ex...</t>
+  </si>
+  <si>
+    <t>src\dc\format_example.json</t>
+  </si>
+  <si>
+    <t>(Same code twice)</t>
+  </si>
+  <si>
+    <t>added wip imple...</t>
+  </si>
+  <si>
+    <t>added support t...</t>
+  </si>
+  <si>
+    <t>Added demo...</t>
+  </si>
+  <si>
+    <t>src\dc\abstract.py</t>
   </si>
 </sst>
 </file>
@@ -1376,10 +1400,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2799</c:v>
+                  <c:v>2801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1351</c:v>
+                  <c:v>1564</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>316</c:v>
@@ -1718,7 +1742,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1813,10 +1837,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1837,7 +1861,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -2632,7 +2656,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -2721,7 +2745,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3364,10 +3388,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -3441,10 +3465,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.441860465116279</c:v>
+                  <c:v>1.4318181818181819</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5714285714285714</c:v>
+                  <c:v>1.5416666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.6666666666666667</c:v>
@@ -3518,10 +3542,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.418604651162788</c:v>
+                  <c:v>42.477272727272727</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.904761904761905</c:v>
+                  <c:v>20.979166666666668</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>55.666666666666664</c:v>
@@ -4209,10 +4233,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2692</c:v>
+                  <c:v>2676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1345</c:v>
+                  <c:v>1585</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>278</c:v>
@@ -4317,9 +4341,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -4331,13 +4355,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Last 6</a:t>
+              <a:t>Last 12 commits</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> commits</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4354,9 +4373,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -4385,12 +4404,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4405,12 +4428,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4425,12 +4452,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4445,12 +4476,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4465,12 +4500,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4478,6 +4517,59 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Tätigkeitsdokumentation!$I$2:$M$2</c:f>
@@ -4508,10 +4600,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>67</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4532,11 +4624,12 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
-          <c:showCatName val="0"/>
+          <c:showCatName val="1"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -4554,7 +4647,11 @@
       <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4567,7 +4664,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -4593,12 +4690,19 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -4646,9 +4750,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -4660,17 +4764,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Last 14</a:t>
+              <a:t>Last 14 commits per person </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> commits per person</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4687,9 +4782,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -4718,12 +4813,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4738,12 +4837,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4758,12 +4861,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4778,12 +4885,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4798,12 +4909,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4811,6 +4926,59 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Tätigkeitsdokumentation!$I$2:$M$2</c:f>
@@ -4841,10 +5009,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>816</c:v>
+                  <c:v>799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>465</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>316</c:v>
@@ -4865,11 +5033,12 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
-          <c:showCatName val="0"/>
+          <c:showCatName val="1"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -4887,7 +5056,11 @@
       <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4900,7 +5073,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -4926,12 +5099,19 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -7779,56 +7959,52 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -7843,12 +8019,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -7862,9 +8035,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
@@ -7880,36 +8055,51 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -7919,7 +8109,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -7931,25 +8121,26 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -7957,7 +8148,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -7973,7 +8164,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -7982,7 +8173,7 @@
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -7997,7 +8188,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8008,7 +8199,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8022,12 +8213,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8041,12 +8232,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8060,7 +8251,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:noFill/>
@@ -8074,12 +8265,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -8093,12 +8284,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -8112,12 +8303,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
@@ -8131,12 +8322,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8150,11 +8341,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
@@ -8162,7 +8360,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -8170,7 +8368,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -8178,7 +8376,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8190,12 +8388,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8209,12 +8407,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -8223,14 +8421,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -8239,7 +8437,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8251,7 +8449,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8259,7 +8457,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8273,7 +8471,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8285,69 +8483,59 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -8362,12 +8550,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -8381,9 +8566,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
@@ -8399,36 +8586,51 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -8438,7 +8640,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -8450,25 +8652,26 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -8476,7 +8679,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8492,7 +8695,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8501,7 +8704,7 @@
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -8516,7 +8719,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8527,7 +8730,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8541,12 +8744,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8560,12 +8763,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8579,7 +8782,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:noFill/>
@@ -8593,12 +8796,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -8612,12 +8815,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -8631,12 +8834,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
@@ -8650,12 +8853,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8669,11 +8872,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
@@ -8681,7 +8891,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -8689,7 +8899,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -8697,7 +8907,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8709,12 +8919,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -8728,12 +8938,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -8742,14 +8952,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -8758,7 +8968,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8770,7 +8980,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8778,7 +8988,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -8792,7 +9002,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -8804,14 +9014,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -8821,15 +9025,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>8473</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>6774</xdr:rowOff>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>598715</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>358589</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>187017</xdr:rowOff>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8856,16 +9060,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>180415</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>44825</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>101973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>220</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>560295</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>125666</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8892,16 +9096,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>38420</xdr:colOff>
-      <xdr:row>221</xdr:row>
-      <xdr:rowOff>5920</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>565096</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>117979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>374596</xdr:colOff>
-      <xdr:row>235</xdr:row>
-      <xdr:rowOff>82120</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1199029</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>3679</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8928,16 +9132,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1868261</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>87087</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>8646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>163287</xdr:rowOff>
+      <xdr:colOff>1220881</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>84846</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8964,16 +9168,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1866901</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>140154</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>17931</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>16890</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1208315</xdr:colOff>
-      <xdr:row>233</xdr:row>
-      <xdr:rowOff>25854</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>93090</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9000,16 +9204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>605116</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>200</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>605116</xdr:colOff>
-      <xdr:row>186</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>12606</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9037,15 +9241,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>20449</xdr:colOff>
-      <xdr:row>157</xdr:row>
-      <xdr:rowOff>61352</xdr:rowOff>
+      <xdr:colOff>31655</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>5322</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>139233</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>33617</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>83203</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9396,8 +9600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G205" sqref="G205:M232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13481,20 +13685,37 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B95" s="7"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="8"/>
+      <c r="A95" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" s="17">
+        <v>87</v>
+      </c>
+      <c r="E95" s="17">
+        <v>1</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>186</v>
+      </c>
       <c r="I95">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J95">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="K95">
         <f t="shared" si="6"/>
@@ -13509,20 +13730,37 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B96" s="7"/>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="8"/>
+      <c r="A96" t="s">
+        <v>128</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D96" s="17">
+        <v>8</v>
+      </c>
+      <c r="E96" s="17">
+        <v>1</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="I96">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J96">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K96">
         <f t="shared" si="6"/>
@@ -13536,13 +13774,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B97" s="7"/>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="16"/>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="17">
+        <v>20</v>
+      </c>
+      <c r="E97" s="17">
+        <v>2</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H97" s="8"/>
       <c r="I97">
         <f t="shared" si="6"/>
@@ -13550,7 +13803,7 @@
       </c>
       <c r="J97">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K97">
         <f t="shared" si="6"/>
@@ -13564,13 +13817,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B98" s="7"/>
-      <c r="C98" s="16"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="16"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="16"/>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>128</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D98" s="17">
+        <v>24</v>
+      </c>
+      <c r="E98" s="17">
+        <v>1</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G98" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H98" s="8"/>
       <c r="I98">
         <f t="shared" si="6"/>
@@ -13578,7 +13846,7 @@
       </c>
       <c r="J98">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K98">
         <f t="shared" si="6"/>
@@ -13592,13 +13860,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B99" s="7"/>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="16"/>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99" s="17">
+        <v>22</v>
+      </c>
+      <c r="E99" s="17">
+        <v>2</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H99" s="8"/>
       <c r="I99">
         <f t="shared" si="6"/>
@@ -13606,7 +13889,7 @@
       </c>
       <c r="J99">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="K99">
         <f t="shared" si="6"/>
@@ -13620,17 +13903,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B100" s="7"/>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
-      <c r="G100" s="16"/>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D100" s="17">
+        <v>2</v>
+      </c>
+      <c r="E100" s="17">
+        <v>1</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G100" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="H100" s="8"/>
       <c r="I100">
         <f t="shared" ref="I100:L115" si="7">MAX(0, IF($G100=I$2, $D100*$E100, 0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J100">
         <f t="shared" si="7"/>
@@ -13648,13 +13946,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B101" s="7"/>
-      <c r="C101" s="16"/>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="16"/>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>128</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="17">
+        <v>10</v>
+      </c>
+      <c r="E101" s="17">
+        <v>1</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G101" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="H101" s="8"/>
       <c r="I101">
         <f t="shared" si="7"/>
@@ -13662,7 +13975,7 @@
       </c>
       <c r="J101">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K101">
         <f t="shared" si="7"/>
@@ -13676,7 +13989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
@@ -13704,7 +14017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B103" s="7"/>
       <c r="C103" s="16"/>
       <c r="D103" s="16"/>
@@ -13732,7 +14045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
       <c r="C104" s="16"/>
       <c r="D104" s="16"/>
@@ -13760,7 +14073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
       <c r="C105" s="16"/>
       <c r="D105" s="16"/>
@@ -13788,7 +14101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
       <c r="C106" s="16"/>
       <c r="D106" s="16"/>
@@ -13816,7 +14129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B107" s="7"/>
       <c r="C107" s="16"/>
       <c r="D107" s="16"/>
@@ -13844,7 +14157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B108" s="7"/>
       <c r="C108" s="16"/>
       <c r="D108" s="16"/>
@@ -13872,7 +14185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B109" s="7"/>
       <c r="C109" s="16"/>
       <c r="D109" s="16"/>
@@ -13900,7 +14213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B110" s="7"/>
       <c r="C110" s="16"/>
       <c r="D110" s="16"/>
@@ -13928,7 +14241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B111" s="7"/>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
@@ -13956,7 +14269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B112" s="7"/>
       <c r="C112" s="16"/>
       <c r="D112" s="16"/>
@@ -16475,11 +16788,11 @@
       </c>
       <c r="I201" s="10">
         <f>SUM(I$3:I$200)</f>
-        <v>2799</v>
+        <v>2801</v>
       </c>
       <c r="J201" s="10">
         <f>SUM(J$3:J$200)</f>
-        <v>1351</v>
+        <v>1564</v>
       </c>
       <c r="K201" s="10">
         <f>SUM(K$3:K$200)</f>
@@ -16499,15 +16812,15 @@
         <v>182</v>
       </c>
       <c r="H202">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I202" s="17" cm="1">
         <f t="array" ref="I202">SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (ROW(I$3:I$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(I$3:I$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J202" s="17" cm="1">
         <f t="array" ref="J202">SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (ROW(J$3:J$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(J$3:J$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="K202" s="17" cm="1">
         <f t="array" ref="K202">SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (ROW(K$3:K$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(K$3:K$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
@@ -16531,11 +16844,11 @@
       </c>
       <c r="I203" cm="1">
         <f t="array" ref="I203">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0) * (ROW(I$3:I$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0), ROW(I$3:I$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", I$3:I$200, "&gt;0")))))), 0)</f>
-        <v>816</v>
+        <v>799</v>
       </c>
       <c r="J203" cm="1">
         <f t="array" ref="J203">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0) * (ROW(J$3:J$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0), ROW(J$3:J$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", J$3:J$200, "&gt;0")))))), 0)</f>
-        <v>465</v>
+        <v>407</v>
       </c>
       <c r="K203" cm="1">
         <f t="array" ref="K203">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0) * (ROW(K$3:K$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0), ROW(K$3:K$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", K$3:K$200, "&gt;0")))))), 0)</f>
@@ -16556,7 +16869,7 @@
         <v>adalfarus</v>
       </c>
       <c r="J204" t="str">
-        <f t="shared" ref="J204:M204" si="10">J$2</f>
+        <f t="shared" ref="J204:M205" si="10">J$2</f>
         <v>Giesbrt</v>
       </c>
       <c r="K204" t="str">
@@ -16578,11 +16891,11 @@
       </c>
       <c r="I205">
         <f>COUNTIF($G$3:$G$200, I$2)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J205">
         <f>COUNTIF($G$3:$G$200, J$2)</f>
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="K205">
         <f>COUNTIF($G$3:$G$200, K$2)</f>
@@ -16603,11 +16916,11 @@
       </c>
       <c r="I206">
         <f>IF(COUNTIF($G$3:$G$200, I$2) &gt; 0, AVERAGEIF($G$3:$G$200, I$2, $E$3:$E$200), 0)</f>
-        <v>1.441860465116279</v>
+        <v>1.4318181818181819</v>
       </c>
       <c r="J206">
         <f>IF(COUNTIF($G$3:$G$200, J$2) &gt; 0, AVERAGEIF($G$3:$G$200, J$2, $E$3:$E$200), 0)</f>
-        <v>1.5714285714285714</v>
+        <v>1.5416666666666667</v>
       </c>
       <c r="K206">
         <f>IF(COUNTIF($G$3:$G$200, K$2) &gt; 0, AVERAGEIF($G$3:$G$200, K$2, $E$3:$E$200), 0)</f>
@@ -16628,11 +16941,11 @@
       </c>
       <c r="I207">
         <f>IF(COUNTIF($G$3:$G$200, I$2) &gt; 0, AVERAGEIF($G$3:$G$200, I$2, $D$3:$D$200), 0)</f>
-        <v>43.418604651162788</v>
+        <v>42.477272727272727</v>
       </c>
       <c r="J207">
         <f>IF(COUNTIF($G$3:$G$200, J$2) &gt; 0, AVERAGEIF($G$3:$G$200, J$2, $D$3:$D$200), 0)</f>
-        <v>19.904761904761905</v>
+        <v>20.979166666666668</v>
       </c>
       <c r="K207">
         <f>IF(COUNTIF($G$3:$G$200, K$2) &gt; 0, AVERAGEIF($G$3:$G$200, K$2, $D$3:$D$200), 0)</f>
@@ -16653,11 +16966,11 @@
       </c>
       <c r="I208">
         <f>ROUND(I$205*I$206*I$207, 0)</f>
-        <v>2692</v>
+        <v>2676</v>
       </c>
       <c r="J208">
         <f>ROUND(J$205*J$206*J$207, 0)</f>
-        <v>1345</v>
+        <v>1585</v>
       </c>
       <c r="K208">
         <f>ROUND(K$205*K$206*K$207, 0)</f>
@@ -16681,7 +16994,7 @@
         <v>adalfarus</v>
       </c>
       <c r="J210" t="str">
-        <f t="shared" ref="J210:M210" si="11">J$2</f>
+        <f t="shared" ref="J210:M211" si="11">J$2</f>
         <v>Giesbrt</v>
       </c>
       <c r="K210" t="str">
@@ -16703,19 +17016,19 @@
         <v>everything</v>
       </c>
       <c r="I211">
-        <f t="shared" ref="I211:L222" si="12">COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G211)</f>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G211)</f>
         <v>12</v>
       </c>
       <c r="J211">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G211)</f>
+        <v>16</v>
       </c>
       <c r="K211">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G211)</f>
         <v>3</v>
       </c>
       <c r="L211">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G211)</f>
         <v>0</v>
       </c>
       <c r="M211">
@@ -16728,23 +17041,23 @@
         <v>changes</v>
       </c>
       <c r="I212">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G212)</f>
         <v>17</v>
       </c>
       <c r="J212">
-        <f t="shared" si="12"/>
-        <v>13</v>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G212)</f>
+        <v>15</v>
       </c>
       <c r="K212">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G212)</f>
         <v>0</v>
       </c>
       <c r="L212">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G212)</f>
         <v>2</v>
       </c>
       <c r="M212">
-        <f t="shared" ref="M212:M222" si="13">COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G212)</f>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G212)</f>
         <v>0</v>
       </c>
     </row>
@@ -16753,23 +17066,23 @@
         <v>new cls</v>
       </c>
       <c r="I213">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G213)</f>
         <v>1</v>
       </c>
       <c r="J213">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G213)</f>
         <v>0</v>
       </c>
       <c r="K213">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G213)</f>
         <v>0</v>
       </c>
       <c r="L213">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G213)</f>
         <v>0</v>
       </c>
       <c r="M213">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G213)</f>
         <v>0</v>
       </c>
     </row>
@@ -16778,23 +17091,23 @@
         <v>docs</v>
       </c>
       <c r="I214">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G214)</f>
         <v>1</v>
       </c>
       <c r="J214">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G214)</f>
         <v>5</v>
       </c>
       <c r="K214">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G214)</f>
         <v>0</v>
       </c>
       <c r="L214">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G214)</f>
         <v>0</v>
       </c>
       <c r="M214">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G214)</f>
         <v>0</v>
       </c>
     </row>
@@ -16803,23 +17116,23 @@
         <v>change docs</v>
       </c>
       <c r="I215">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G215)</f>
         <v>0</v>
       </c>
       <c r="J215">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G215)</f>
         <v>3</v>
       </c>
       <c r="K215">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G215)</f>
         <v>0</v>
       </c>
       <c r="L215">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G215)</f>
         <v>0</v>
       </c>
       <c r="M215">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G215)</f>
         <v>0</v>
       </c>
     </row>
@@ -16828,23 +17141,23 @@
         <v>remove</v>
       </c>
       <c r="I216">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G216)</f>
         <v>1</v>
       </c>
       <c r="J216">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G216)</f>
         <v>0</v>
       </c>
       <c r="K216">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G216)</f>
         <v>0</v>
       </c>
       <c r="L216">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G216)</f>
         <v>0</v>
       </c>
       <c r="M216">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G216)</f>
         <v>0</v>
       </c>
     </row>
@@ -16853,23 +17166,23 @@
         <v>created</v>
       </c>
       <c r="I217">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G217)</f>
         <v>1</v>
       </c>
       <c r="J217">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G217)</f>
         <v>0</v>
       </c>
       <c r="K217">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G217)</f>
         <v>0</v>
       </c>
       <c r="L217">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G217)</f>
         <v>0</v>
       </c>
       <c r="M217">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G217)</f>
         <v>0</v>
       </c>
     </row>
@@ -16878,23 +17191,23 @@
         <v>smaller updates</v>
       </c>
       <c r="I218">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G218)</f>
         <v>1</v>
       </c>
       <c r="J218">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G218)</f>
         <v>1</v>
       </c>
       <c r="K218">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G218)</f>
         <v>0</v>
       </c>
       <c r="L218">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G218)</f>
         <v>0</v>
       </c>
       <c r="M218">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G218)</f>
         <v>0</v>
       </c>
     </row>
@@ -16903,23 +17216,23 @@
         <v>added</v>
       </c>
       <c r="I219">
-        <f t="shared" si="12"/>
-        <v>8</v>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G219)</f>
+        <v>9</v>
       </c>
       <c r="J219">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G219)</f>
+        <v>7</v>
       </c>
       <c r="K219">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G219)</f>
         <v>0</v>
       </c>
       <c r="L219">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G219)</f>
         <v>0</v>
       </c>
       <c r="M219">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G219)</f>
         <v>0</v>
       </c>
     </row>
@@ -16928,23 +17241,23 @@
         <v>setter</v>
       </c>
       <c r="I220">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G220)</f>
         <v>0</v>
       </c>
       <c r="J220">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G220)</f>
         <v>1</v>
       </c>
       <c r="K220">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G220)</f>
         <v>0</v>
       </c>
       <c r="L220">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G220)</f>
         <v>0</v>
       </c>
       <c r="M220">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G220)</f>
         <v>0</v>
       </c>
     </row>
@@ -16953,23 +17266,23 @@
         <v>moved</v>
       </c>
       <c r="I221">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G221)</f>
         <v>0</v>
       </c>
       <c r="J221">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G221)</f>
         <v>1</v>
       </c>
       <c r="K221">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G221)</f>
         <v>0</v>
       </c>
       <c r="L221">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G221)</f>
         <v>0</v>
       </c>
       <c r="M221">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G221)</f>
         <v>0</v>
       </c>
     </row>
@@ -16978,23 +17291,23 @@
         <v>fixes</v>
       </c>
       <c r="I222">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G222)</f>
         <v>1</v>
       </c>
       <c r="J222">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, J$210, $C$3:$C$200, $G222)</f>
         <v>0</v>
       </c>
       <c r="K222">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, K$210, $C$3:$C$200, $G222)</f>
         <v>0</v>
       </c>
       <c r="L222">
-        <f t="shared" si="12"/>
+        <f>COUNTIFS($G$3:$G$200, L$210, $C$3:$C$200, $G222)</f>
         <v>0</v>
       </c>
       <c r="M222">
-        <f t="shared" si="13"/>
+        <f>COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G222)</f>
         <v>0</v>
       </c>
     </row>
@@ -17003,23 +17316,23 @@
         <v>170</v>
       </c>
       <c r="I224" t="str">
-        <f t="shared" ref="I224:M224" si="14">I$2</f>
+        <f t="shared" ref="I224:M225" si="12">I$2</f>
         <v>adalfarus</v>
       </c>
       <c r="J224" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Giesbrt</v>
       </c>
       <c r="K224" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Fa4953</v>
       </c>
       <c r="L224" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>TheCodeJak</v>
       </c>
       <c r="M224" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>XXXXXX</v>
       </c>
     </row>
@@ -17029,23 +17342,23 @@
         <v>none</v>
       </c>
       <c r="I225">
-        <f t="shared" ref="I225:M231" si="15">COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G225)</f>
-        <v>30</v>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G225)</f>
+        <v>31</v>
       </c>
       <c r="J225">
-        <f t="shared" si="15"/>
-        <v>19</v>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G225)</f>
+        <v>25</v>
       </c>
       <c r="K225">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G225)</f>
         <v>0</v>
       </c>
       <c r="L225">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G225)</f>
         <v>2</v>
       </c>
       <c r="M225">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G225)</f>
         <v>0</v>
       </c>
     </row>
@@ -17054,23 +17367,23 @@
         <v>comments 5%</v>
       </c>
       <c r="I226">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G226)</f>
         <v>2</v>
       </c>
       <c r="J226">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G226)</f>
         <v>0</v>
       </c>
       <c r="K226">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G226)</f>
         <v>0</v>
       </c>
       <c r="L226">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G226)</f>
         <v>0</v>
       </c>
       <c r="M226">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G226)</f>
         <v>0</v>
       </c>
     </row>
@@ -17079,23 +17392,23 @@
         <v>inline 100%</v>
       </c>
       <c r="I227">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G227)</f>
         <v>6</v>
       </c>
       <c r="J227">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G227)</f>
         <v>23</v>
       </c>
       <c r="K227">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G227)</f>
         <v>3</v>
       </c>
       <c r="L227">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G227)</f>
         <v>0</v>
       </c>
       <c r="M227">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G227)</f>
         <v>0</v>
       </c>
     </row>
@@ -17104,23 +17417,23 @@
         <v>inline 5%</v>
       </c>
       <c r="I228">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G228)</f>
         <v>3</v>
       </c>
       <c r="J228">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G228)</f>
         <v>0</v>
       </c>
       <c r="K228">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G228)</f>
         <v>0</v>
       </c>
       <c r="L228">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G228)</f>
         <v>0</v>
       </c>
       <c r="M228">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G228)</f>
         <v>0</v>
       </c>
     </row>
@@ -17129,23 +17442,23 @@
         <v>comments 100%</v>
       </c>
       <c r="I229">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G229)</f>
         <v>1</v>
       </c>
       <c r="J229">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G229)</f>
         <v>0</v>
       </c>
       <c r="K229">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G229)</f>
         <v>0</v>
       </c>
       <c r="L229">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G229)</f>
         <v>0</v>
       </c>
       <c r="M229">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G229)</f>
         <v>0</v>
       </c>
     </row>
@@ -17154,23 +17467,23 @@
         <v>inline 50%</v>
       </c>
       <c r="I230">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G230)</f>
         <v>0</v>
       </c>
       <c r="J230">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G230)</f>
         <v>1</v>
       </c>
       <c r="K230">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G230)</f>
         <v>0</v>
       </c>
       <c r="L230">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G230)</f>
         <v>0</v>
       </c>
       <c r="M230">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G230)</f>
         <v>0</v>
       </c>
     </row>
@@ -17179,23 +17492,23 @@
         <v>in md 100%</v>
       </c>
       <c r="I231">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, I$224, $F$3:$F$200, $G231)</f>
         <v>1</v>
       </c>
       <c r="J231">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, J$224, $F$3:$F$200, $G231)</f>
         <v>0</v>
       </c>
       <c r="K231">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, K$224, $F$3:$F$200, $G231)</f>
         <v>0</v>
       </c>
       <c r="L231">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, L$224, $F$3:$F$200, $G231)</f>
         <v>0</v>
       </c>
       <c r="M231">
-        <f t="shared" si="15"/>
+        <f>COUNTIFS($G$3:$G$200, M$224, $F$3:$F$200, $G231)</f>
         <v>0</v>
       </c>
     </row>
@@ -17257,10 +17570,14 @@
     <hyperlink ref="A92" r:id="rId51" location="diff-637e49ef799bb51094751e67276f1dfeaeb31048cd7e0de7c90fef139d184c88" xr:uid="{DE70295C-A534-4238-99A2-20844BBF02B2}"/>
     <hyperlink ref="A93" r:id="rId52" location="diff-acc8dd38fd22df5f73d37cc21057624272a3b57ca4a77619f6222bb7324d835b" xr:uid="{30211D90-6DDF-46BC-AF51-A4937D04B7CD}"/>
     <hyperlink ref="A94" r:id="rId53" location="diff-4d7c51b1efe9043e44439a949dfd92e5827321b34082903477fd04876edb7552" xr:uid="{7B32070D-3F21-419E-A4AE-CB0FFCC800B3}"/>
+    <hyperlink ref="A95" r:id="rId54" xr:uid="{B9C706A2-12AB-4191-8154-6AF0FF26E6D0}"/>
+    <hyperlink ref="A97" r:id="rId55" location="diff-e4f12f881ad46f5c2645b7d2e7e1481c2d02260597fe5c21bf0a896acf246f67" xr:uid="{E5FB0512-E9D9-43DF-978D-FA39B56D828B}"/>
+    <hyperlink ref="A99" r:id="rId56" location="diff-7193f7df8c6f35c6f42d6f9db6deb3bf3d1a1000927552b84c901eca5b9b37e0" xr:uid="{0D67263D-DC79-443B-AEB8-164521F1F2B6}"/>
+    <hyperlink ref="A100" r:id="rId57" location="diff-745b76dfac54a92f874117e7c871c43517832e1c7317878f6a2c27dcd02833d8" xr:uid="{1B5DCDBC-927B-42E7-BCCE-46B9D37A3D60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId54"/>
-  <drawing r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId58"/>
+  <drawing r:id="rId59"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Extended commit table and made it more dynamic
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/CommitTable.xlsx
+++ b/meta/dudpy-planning/CommitTable.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E02E6-F894-4F83-B543-8CD7428EBEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DBEA1F-E501-47A8-8459-9A7987740F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="254">
   <si>
     <t>Datei</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>added field "id" ...</t>
+  </si>
+  <si>
+    <t>Rows:</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1061,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1090,11 +1093,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1112,7 +1116,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1580,7 +1584,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$201:$M$201</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$301:$M$301</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1675,7 +1679,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1753,7 +1757,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$210</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$310</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1774,7 +1778,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$211:$G$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$311:$G$322</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1818,7 +1822,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$211:$I$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$311:$I$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1872,7 +1876,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$J$210</c:f>
+              <c:f>Tätigkeitsdokumentation!$J$310</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1893,7 +1897,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$211:$G$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$311:$G$322</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1937,7 +1941,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$J$211:$J$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$J$311:$J$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1991,7 +1995,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$K$210</c:f>
+              <c:f>Tätigkeitsdokumentation!$K$310</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2012,7 +2016,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$211:$G$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$311:$G$322</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2056,7 +2060,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$K$211:$K$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$K$311:$K$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2110,7 +2114,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$L$210</c:f>
+              <c:f>Tätigkeitsdokumentation!$L$310</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2131,7 +2135,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$211:$G$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$311:$G$322</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2175,7 +2179,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$L$211:$L$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$L$311:$L$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2229,7 +2233,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$M$210</c:f>
+              <c:f>Tätigkeitsdokumentation!$M$310</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2250,7 +2254,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$211:$G$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$311:$G$322</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2294,7 +2298,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$M$211:$M$222</c:f>
+              <c:f>Tätigkeitsdokumentation!$M$311:$M$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2563,7 +2567,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2641,7 +2645,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$H$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$H$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -2659,7 +2663,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2688,7 +2692,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$H$226:$H$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$H$326:$H$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2706,7 +2710,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2727,7 +2731,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2756,7 +2760,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$226:$I$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$326:$I$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2795,7 +2799,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$J$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$J$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2816,7 +2820,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2845,7 +2849,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$J$226:$J$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$J$326:$J$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2884,7 +2888,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$K$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$K$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2905,7 +2909,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2934,7 +2938,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$K$226:$K$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$K$326:$K$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2973,7 +2977,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$L$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$L$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2994,7 +2998,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -3023,7 +3027,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$L$226:$L$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$L$326:$L$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3062,7 +3066,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$M$225</c:f>
+              <c:f>Tätigkeitsdokumentation!$M$325</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3083,7 +3087,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$226:$G$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$326:$G$332</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -3112,7 +3116,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$M$226:$M$232</c:f>
+              <c:f>Tätigkeitsdokumentation!$M$326:$M$332</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3366,7 +3370,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3444,7 +3448,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$205:$H$205</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$305:$H$305</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -3465,7 +3469,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$204:$M$204</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$304:$M$304</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3488,7 +3492,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$205:$M$205</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$305:$M$305</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3521,7 +3525,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$206:$H$206</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$306:$H$306</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -3542,7 +3546,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$204:$M$204</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$304:$M$304</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3565,7 +3569,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$206:$M$206</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$306:$M$306</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3598,7 +3602,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$207:$H$207</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$307:$H$307</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -3619,7 +3623,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$204:$M$204</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$304:$M$304</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3642,7 +3646,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$207:$M$207</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$307:$M$307</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3889,7 +3893,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3940,7 +3944,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$G$208:$H$208</c:f>
+              <c:f>Tätigkeitsdokumentation!$G$308:$H$308</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -4310,7 +4314,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$204:$M$204</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$304:$M$304</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4333,7 +4337,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$208:$M$208</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$308:$M$308</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4428,7 +4432,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4700,7 +4704,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$202:$M$202</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$302:$M$302</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4837,7 +4841,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5109,7 +5113,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$203:$M$203</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$303:$M$303</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5246,7 +5250,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5478,7 +5482,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tätigkeitsdokumentation!$I$238:$M$238</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$335:$M$335</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5501,7 +5505,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tätigkeitsdokumentation!$I$239:$M$239</c:f>
+              <c:f>Tätigkeitsdokumentation!$I$336:$M$336</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -10070,15 +10074,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>186</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:colOff>5604</xdr:colOff>
+      <xdr:row>300</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>453838</xdr:colOff>
-      <xdr:row>200</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:colOff>364192</xdr:colOff>
+      <xdr:row>314</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10107,13 +10111,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>44825</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>315</xdr:row>
       <xdr:rowOff>101973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>560295</xdr:colOff>
-      <xdr:row>230</xdr:row>
+      <xdr:row>330</xdr:row>
       <xdr:rowOff>125666</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10143,13 +10147,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>565096</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>315</xdr:row>
       <xdr:rowOff>117979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1199029</xdr:colOff>
-      <xdr:row>230</xdr:row>
+      <xdr:row>330</xdr:row>
       <xdr:rowOff>3679</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10179,13 +10183,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>549088</xdr:colOff>
-      <xdr:row>201</xdr:row>
+      <xdr:row>301</xdr:row>
       <xdr:rowOff>8646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1220881</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>315</xdr:row>
       <xdr:rowOff>84846</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10214,15 +10218,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>17931</xdr:colOff>
-      <xdr:row>201</xdr:row>
-      <xdr:rowOff>16890</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>300</xdr:row>
+      <xdr:rowOff>184978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>537882</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>93090</xdr:rowOff>
+      <xdr:colOff>519951</xdr:colOff>
+      <xdr:row>315</xdr:row>
+      <xdr:rowOff>59472</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10250,15 +10254,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>200</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>5604</xdr:colOff>
+      <xdr:row>314</xdr:row>
+      <xdr:rowOff>125226</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>12606</xdr:rowOff>
+      <xdr:colOff>5604</xdr:colOff>
+      <xdr:row>328</xdr:row>
+      <xdr:rowOff>180695</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10286,15 +10290,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>126904</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>5322</xdr:rowOff>
+      <xdr:colOff>37258</xdr:colOff>
+      <xdr:row>328</xdr:row>
+      <xdr:rowOff>173411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>128866</xdr:colOff>
-      <xdr:row>229</xdr:row>
-      <xdr:rowOff>83203</xdr:rowOff>
+      <xdr:colOff>39220</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>60792</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10322,15 +10326,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>118459</xdr:colOff>
-      <xdr:row>229</xdr:row>
-      <xdr:rowOff>97970</xdr:rowOff>
+      <xdr:colOff>28813</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>75559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>240</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
+      <xdr:colOff>60033</xdr:colOff>
+      <xdr:row>354</xdr:row>
+      <xdr:rowOff>127268</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10359,9 +10363,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -10399,9 +10403,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10434,9 +10438,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10469,9 +10490,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -10645,13 +10683,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M239"/>
+  <dimension ref="A1:N336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J227" sqref="J227"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H339" sqref="H339"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
@@ -10673,6 +10711,12 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
+      <c r="E1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1">
+        <v>300</v>
+      </c>
       <c r="H1" s="12" t="s">
         <v>13</v>
       </c>
@@ -18715,7 +18759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B193" s="7"/>
       <c r="H193" s="8"/>
       <c r="I193">
@@ -18731,14 +18775,14 @@
         <v>0</v>
       </c>
       <c r="L193">
-        <f t="shared" ref="I193:L200" si="3">MAX(0, IF($G193=L$2, $D193*$E193, 0))</f>
+        <f t="shared" ref="I193:L208" si="3">MAX(0, IF($G193=L$2, $D193*$E193, 0))</f>
         <v>0</v>
       </c>
       <c r="M193" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B194" s="7"/>
       <c r="H194" s="8"/>
       <c r="I194">
@@ -18761,7 +18805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B195" s="7"/>
       <c r="H195" s="8"/>
       <c r="I195">
@@ -18784,7 +18828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B196" s="7"/>
       <c r="H196" s="8"/>
       <c r="I196">
@@ -18807,7 +18851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B197" s="7"/>
       <c r="H197" s="8"/>
       <c r="I197">
@@ -18830,7 +18874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B198" s="7"/>
       <c r="H198" s="8"/>
       <c r="I198">
@@ -18853,7 +18897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B199" s="7"/>
       <c r="H199" s="8"/>
       <c r="I199">
@@ -18876,7 +18920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B200" s="7"/>
       <c r="H200" s="8"/>
       <c r="I200">
@@ -18892,817 +18936,3118 @@
         <v>0</v>
       </c>
       <c r="L200">
-        <f t="shared" ref="L200" si="4">MAX(0, IF($G200=L$2, $D200*$E200, 0))</f>
+        <f t="shared" ref="L200:L263" si="4">MAX(0, IF($G200=L$2, $D200*$E200, 0))</f>
         <v>0</v>
       </c>
       <c r="M200" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="10" t="s">
+    <row r="201" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B201" s="7"/>
+      <c r="H201" s="8"/>
+      <c r="I201">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J201">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K201">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L201">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M201" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B202" s="7"/>
+      <c r="H202" s="8"/>
+      <c r="I202">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J202">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K202">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L202">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M202" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B203" s="7"/>
+      <c r="H203" s="8"/>
+      <c r="I203">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K203">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L203">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M203" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B204" s="7"/>
+      <c r="H204" s="8"/>
+      <c r="I204">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K204">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L204">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M204" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B205" s="7"/>
+      <c r="H205" s="8"/>
+      <c r="I205">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K205">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L205">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M205" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B206" s="7"/>
+      <c r="H206" s="8"/>
+      <c r="I206">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K206">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L206">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M206" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B207" s="7"/>
+      <c r="H207" s="8"/>
+      <c r="I207">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K207">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L207">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M207" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B208" s="7"/>
+      <c r="H208" s="8"/>
+      <c r="I208">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K208">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L208">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M208" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B209" s="7"/>
+      <c r="H209" s="8"/>
+      <c r="I209">
+        <f t="shared" ref="I209:L272" si="5">MAX(0, IF($G209=I$2, $D209*$E209, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K209">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L209">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M209" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B210" s="7"/>
+      <c r="H210" s="8"/>
+      <c r="I210">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J210">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K210">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L210">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M210" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B211" s="7"/>
+      <c r="H211" s="8"/>
+      <c r="I211">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J211">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K211">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L211">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M211" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B212" s="7"/>
+      <c r="H212" s="8"/>
+      <c r="I212">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J212">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K212">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L212">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M212" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B213" s="7"/>
+      <c r="H213" s="8"/>
+      <c r="I213">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J213">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K213">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L213">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M213" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B214" s="7"/>
+      <c r="H214" s="8"/>
+      <c r="I214">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J214">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K214">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L214">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M214" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B215" s="7"/>
+      <c r="H215" s="8"/>
+      <c r="I215">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J215">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K215">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L215">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M215" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B216" s="7"/>
+      <c r="H216" s="8"/>
+      <c r="I216">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J216">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K216">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L216">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M216" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B217" s="7"/>
+      <c r="H217" s="8"/>
+      <c r="I217">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J217">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K217">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L217">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M217" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B218" s="7"/>
+      <c r="H218" s="8"/>
+      <c r="I218">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J218">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K218">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L218">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M218" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B219" s="7"/>
+      <c r="H219" s="8"/>
+      <c r="I219">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J219">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K219">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L219">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M219" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B220" s="7"/>
+      <c r="H220" s="8"/>
+      <c r="I220">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J220">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K220">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L220">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M220" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B221" s="7"/>
+      <c r="H221" s="8"/>
+      <c r="I221">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J221">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K221">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L221">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M221" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B222" s="7"/>
+      <c r="H222" s="8"/>
+      <c r="I222">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J222">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K222">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L222">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M222" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B223" s="7"/>
+      <c r="H223" s="8"/>
+      <c r="I223">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J223">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K223">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L223">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M223" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B224" s="7"/>
+      <c r="H224" s="8"/>
+      <c r="I224">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J224">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K224">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L224">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M224" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B225" s="7"/>
+      <c r="H225" s="8"/>
+      <c r="I225">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J225">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K225">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L225">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M225" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B226" s="7"/>
+      <c r="H226" s="8"/>
+      <c r="I226">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J226">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K226">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L226">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M226" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B227" s="7"/>
+      <c r="H227" s="8"/>
+      <c r="I227">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J227">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K227">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L227">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M227" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B228" s="7"/>
+      <c r="H228" s="8"/>
+      <c r="I228">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J228">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K228">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L228">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M228" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B229" s="7"/>
+      <c r="H229" s="8"/>
+      <c r="I229">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J229">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K229">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L229">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M229" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B230" s="7"/>
+      <c r="H230" s="8"/>
+      <c r="I230">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J230">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K230">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L230">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M230" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B231" s="7"/>
+      <c r="H231" s="8"/>
+      <c r="I231">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J231">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K231">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L231">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M231" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B232" s="7"/>
+      <c r="H232" s="8"/>
+      <c r="I232">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J232">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K232">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L232">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M232" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B233" s="7"/>
+      <c r="H233" s="8"/>
+      <c r="I233">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J233">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K233">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L233">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M233" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B234" s="7"/>
+      <c r="H234" s="8"/>
+      <c r="I234">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J234">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K234">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L234">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M234" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B235" s="7"/>
+      <c r="H235" s="8"/>
+      <c r="I235">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J235">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K235">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L235">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M235" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B236" s="7"/>
+      <c r="H236" s="8"/>
+      <c r="I236">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J236">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K236">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L236">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M236" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B237" s="7"/>
+      <c r="H237" s="8"/>
+      <c r="I237">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J237">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K237">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L237">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M237" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B238" s="7"/>
+      <c r="H238" s="8"/>
+      <c r="I238">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J238">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K238">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L238">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M238" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B239" s="7"/>
+      <c r="H239" s="8"/>
+      <c r="I239">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J239">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K239">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L239">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M239" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B240" s="7"/>
+      <c r="H240" s="8"/>
+      <c r="I240">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J240">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K240">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L240">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M240" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B241" s="7"/>
+      <c r="H241" s="8"/>
+      <c r="I241">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J241">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K241">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L241">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M241" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B242" s="7"/>
+      <c r="H242" s="8"/>
+      <c r="I242">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J242">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K242">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L242">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M242" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B243" s="7"/>
+      <c r="H243" s="8"/>
+      <c r="I243">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J243">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K243">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L243">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M243" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B244" s="7"/>
+      <c r="H244" s="8"/>
+      <c r="I244">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J244">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K244">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L244">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M244" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B245" s="7"/>
+      <c r="H245" s="8"/>
+      <c r="I245">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J245">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K245">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L245">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M245" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B246" s="7"/>
+      <c r="H246" s="8"/>
+      <c r="I246">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J246">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K246">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L246">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M246" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B247" s="7"/>
+      <c r="H247" s="8"/>
+      <c r="I247">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J247">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K247">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L247">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M247" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B248" s="7"/>
+      <c r="H248" s="8"/>
+      <c r="I248">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J248">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K248">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L248">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M248" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B249" s="7"/>
+      <c r="H249" s="8"/>
+      <c r="I249">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J249">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K249">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L249">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M249" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B250" s="7"/>
+      <c r="H250" s="8"/>
+      <c r="I250">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J250">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K250">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L250">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M250" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B251" s="7"/>
+      <c r="H251" s="8"/>
+      <c r="I251">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J251">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K251">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L251">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M251" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B252" s="7"/>
+      <c r="H252" s="8"/>
+      <c r="I252">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J252">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K252">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L252">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M252" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B253" s="7"/>
+      <c r="H253" s="8"/>
+      <c r="I253">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J253">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K253">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L253">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M253" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B254" s="7"/>
+      <c r="H254" s="8"/>
+      <c r="I254">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J254">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K254">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L254">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M254" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B255" s="7"/>
+      <c r="H255" s="8"/>
+      <c r="I255">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J255">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K255">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L255">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M255" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B256" s="7"/>
+      <c r="H256" s="8"/>
+      <c r="I256">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K256">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L256">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M256" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B257" s="7"/>
+      <c r="H257" s="8"/>
+      <c r="I257">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J257">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K257">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L257">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M257" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B258" s="7"/>
+      <c r="H258" s="8"/>
+      <c r="I258">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K258">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L258">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M258" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B259" s="7"/>
+      <c r="H259" s="8"/>
+      <c r="I259">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K259">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L259">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M259" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B260" s="7"/>
+      <c r="H260" s="8"/>
+      <c r="I260">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K260">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L260">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M260" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B261" s="7"/>
+      <c r="H261" s="8"/>
+      <c r="I261">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K261">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L261">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M261" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B262" s="7"/>
+      <c r="H262" s="8"/>
+      <c r="I262">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K262">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L262">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M262" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B263" s="7"/>
+      <c r="H263" s="8"/>
+      <c r="I263">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K263">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L263">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M263" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B264" s="7"/>
+      <c r="H264" s="8"/>
+      <c r="I264">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J264">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K264">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L264">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M264" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B265" s="7"/>
+      <c r="H265" s="8"/>
+      <c r="I265">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J265">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K265">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L265">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M265" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B266" s="7"/>
+      <c r="H266" s="8"/>
+      <c r="I266">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J266">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K266">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L266">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M266" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B267" s="7"/>
+      <c r="H267" s="8"/>
+      <c r="I267">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J267">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K267">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L267">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M267" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B268" s="7"/>
+      <c r="H268" s="8"/>
+      <c r="I268">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J268">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K268">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L268">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M268" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B269" s="7"/>
+      <c r="H269" s="8"/>
+      <c r="I269">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J269">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K269">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L269">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M269" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B270" s="7"/>
+      <c r="H270" s="8"/>
+      <c r="I270">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J270">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K270">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L270">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M270" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B271" s="7"/>
+      <c r="H271" s="8"/>
+      <c r="I271">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J271">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K271">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L271">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M271" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B272" s="7"/>
+      <c r="H272" s="8"/>
+      <c r="I272">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J272">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K272">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L272">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M272" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B273" s="7"/>
+      <c r="H273" s="8"/>
+      <c r="I273">
+        <f t="shared" ref="I273:L300" si="6">MAX(0, IF($G273=I$2, $D273*$E273, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="J273">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K273">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L273">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M273" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B274" s="7"/>
+      <c r="H274" s="8"/>
+      <c r="I274">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J274">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K274">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L274">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M274" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B275" s="7"/>
+      <c r="H275" s="8"/>
+      <c r="I275">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J275">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K275">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L275">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M275" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B276" s="7"/>
+      <c r="H276" s="8"/>
+      <c r="I276">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J276">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K276">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L276">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M276" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B277" s="7"/>
+      <c r="H277" s="8"/>
+      <c r="I277">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J277">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K277">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L277">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M277" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B278" s="7"/>
+      <c r="H278" s="8"/>
+      <c r="I278">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J278">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K278">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L278">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M278" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B279" s="7"/>
+      <c r="H279" s="8"/>
+      <c r="I279">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J279">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K279">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L279">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M279" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B280" s="7"/>
+      <c r="H280" s="8"/>
+      <c r="I280">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J280">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K280">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L280">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M280" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B281" s="7"/>
+      <c r="H281" s="8"/>
+      <c r="I281">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J281">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K281">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L281">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M281" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B282" s="7"/>
+      <c r="H282" s="8"/>
+      <c r="I282">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J282">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K282">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L282">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M282" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B283" s="7"/>
+      <c r="H283" s="8"/>
+      <c r="I283">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J283">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K283">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L283">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M283" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B284" s="7"/>
+      <c r="H284" s="8"/>
+      <c r="I284">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J284">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K284">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L284">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M284" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B285" s="7"/>
+      <c r="H285" s="8"/>
+      <c r="I285">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J285">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K285">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L285">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M285" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B286" s="7"/>
+      <c r="H286" s="8"/>
+      <c r="I286">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J286">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K286">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L286">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M286" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B287" s="7"/>
+      <c r="H287" s="8"/>
+      <c r="I287">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J287">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K287">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L287">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M287" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B288" s="7"/>
+      <c r="H288" s="8"/>
+      <c r="I288">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J288">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K288">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L288">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M288" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B289" s="7"/>
+      <c r="H289" s="8"/>
+      <c r="I289">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J289">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K289">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L289">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M289" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B290" s="7"/>
+      <c r="H290" s="8"/>
+      <c r="I290">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J290">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K290">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L290">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M290" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B291" s="7"/>
+      <c r="H291" s="8"/>
+      <c r="I291">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J291">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K291">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L291">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M291" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B292" s="7"/>
+      <c r="H292" s="8"/>
+      <c r="I292">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J292">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K292">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L292">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M292" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B293" s="7"/>
+      <c r="H293" s="8"/>
+      <c r="I293">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J293">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K293">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L293">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M293" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B294" s="7"/>
+      <c r="H294" s="8"/>
+      <c r="I294">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J294">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K294">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L294">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M294" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B295" s="7"/>
+      <c r="H295" s="8"/>
+      <c r="I295">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J295">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K295">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L295">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M295" s="8">
+        <v>0</v>
+      </c>
+      <c r="N295" s="19"/>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B296" s="7"/>
+      <c r="H296" s="8"/>
+      <c r="I296">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J296">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K296">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L296">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M296" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B297" s="7"/>
+      <c r="H297" s="8"/>
+      <c r="I297">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J297">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K297">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L297">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M297" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B298" s="7"/>
+      <c r="H298" s="8"/>
+      <c r="I298">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J298">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K298">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L298">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M298" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B299" s="7"/>
+      <c r="H299" s="8"/>
+      <c r="I299">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J299">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K299">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L299">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M299" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B300" s="7"/>
+      <c r="H300" s="8"/>
+      <c r="I300">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J300">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K300">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L300">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M300" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B201" s="9" t="s">
+      <c r="B301" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C201" s="10" t="s">
+      <c r="C301" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D201" s="10" t="s">
+      <c r="D301" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E201" s="10" t="s">
+      <c r="E301" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F201" s="10" t="s">
+      <c r="F301" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G201" s="10" t="s">
+      <c r="G301" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H201" s="11" t="s">
+      <c r="H301" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I201" s="10">
-        <f>SUM(I$3:I$200)</f>
+      <c r="I301" s="10">
+        <f>SUM(I$3:INDEX(I:I,$F$1))</f>
         <v>3833.5</v>
       </c>
-      <c r="J201" s="10">
-        <f>SUM(J$3:J$200)</f>
+      <c r="J301" s="10">
+        <f>SUM(J$3:INDEX(J:J,$F$1))</f>
         <v>3214.5</v>
       </c>
-      <c r="K201" s="10">
-        <f>SUM(K$3:K$200)</f>
+      <c r="K301" s="10">
+        <f>SUM(K$3:INDEX(K:K,$F$1))</f>
         <v>877</v>
       </c>
-      <c r="L201" s="10">
-        <f>SUM(L$3:L$200)</f>
+      <c r="L301" s="10">
+        <f>SUM(L$3:INDEX(L:L,$F$1))</f>
         <v>829</v>
       </c>
-      <c r="M201" s="11">
-        <f>SUM(M$3:M$200)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G202" t="s">
+      <c r="M301" s="10">
+        <f>SUM(M$3:INDEX(M:M,$F$1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G302" t="s">
         <v>181</v>
       </c>
-      <c r="H202">
+      <c r="H302">
         <v>12</v>
       </c>
-      <c r="I202" cm="1">
-        <f t="array" ref="I202">SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (ROW(I$3:I$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(I$3:I$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
+      <c r="I302" cm="1">
+        <f t="array" ref="I302">SUM(_xlfn._xlws.FILTER(I$3:INDEX(I:I,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(I$3:INDEX(I:I,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(I$3:INDEX(I:I,$F$1))), MIN($H$302, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
         <v>18</v>
       </c>
-      <c r="J202" cm="1">
-        <f t="array" ref="J202">SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (ROW(J$3:J$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(J$3:J$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
+      <c r="J302" cm="1">
+        <f t="array" ref="J302">SUM(_xlfn._xlws.FILTER(J$3:INDEX(J:J,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(J$3:INDEX(J:J,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(J$3:INDEX(J:J,$F$1))), MIN($H$302, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
         <v>39</v>
       </c>
-      <c r="K202" cm="1">
-        <f t="array" ref="K202">SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (ROW(K$3:K$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(K$3:K$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
-        <v>0</v>
-      </c>
-      <c r="L202" cm="1">
-        <f t="array" ref="L202">SUM(_xlfn._xlws.FILTER(L$3:L$200, ($G$3:$G$200&lt;&gt;"") * (ROW(L$3:L$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(L$3:L$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
+      <c r="K302" cm="1">
+        <f t="array" ref="K302">SUM(_xlfn._xlws.FILTER(K$3:INDEX(K:K,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(K$3:INDEX(K:K,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(K$3:INDEX(K:K,$F$1))), MIN($H$302, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
+        <v>0</v>
+      </c>
+      <c r="L302" cm="1">
+        <f t="array" ref="L302">SUM(_xlfn._xlws.FILTER(L$3:INDEX(L:L,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(L$3:INDEX(L:L,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(L$3:INDEX(L:L,$F$1))), MIN($H$302, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
         <v>255</v>
       </c>
-      <c r="M202" cm="1">
-        <f t="array" ref="M202">SUM(_xlfn._xlws.FILTER(M$3:M$200, ($G$3:$G$200&lt;&gt;"") * (ROW(M$3:M$200) &gt;= LARGE(IF($G$3:$G$200&lt;&gt;"", ROW(M$3:M$200)), MIN($H$202, COUNTIF($G$3:$G$200, "&lt;&gt;"))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G203" t="s">
+      <c r="M302" cm="1">
+        <f t="array" ref="M302">SUM(_xlfn._xlws.FILTER(M$3:INDEX(M:M,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(M$3:INDEX(M:M,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(M$3:INDEX(M:M,$F$1))), MIN($H$302, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G303" t="s">
         <v>181</v>
       </c>
-      <c r="H203">
+      <c r="H303">
         <v>14</v>
       </c>
-      <c r="I203" cm="1">
-        <f t="array" ref="I203">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:I$200, ($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0) * (ROW(I$3:I$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (I$3:I$200 &gt; 0), ROW(I$3:I$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", I$3:I$200, "&gt;0")))))), 0)</f>
+      <c r="I303" cm="1">
+        <f t="array" ref="I303">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:INDEX(I:I,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (I$3:INDEX(I:I,$F$1) &gt; 0) * (ROW(I$3:INDEX(I:I,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (I$3:INDEX(I:I,$F$1) &gt; 0), ROW(I$3:INDEX(I:I,$F$1))), MIN($H$303, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", I$3:INDEX(I:I,$F$1), "&gt;0")))))), 0)</f>
         <v>1161.5</v>
       </c>
-      <c r="J203" cm="1">
-        <f t="array" ref="J203">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:J$200, ($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0) * (ROW(J$3:J$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (J$3:J$200 &gt; 0), ROW(J$3:J$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", J$3:J$200, "&gt;0")))))), 0)</f>
+      <c r="J303" cm="1">
+        <f t="array" ref="J303">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:INDEX(J:J,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (J$3:INDEX(J:J,$F$1) &gt; 0) * (ROW(J$3:INDEX(J:J,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (J$3:INDEX(J:J,$F$1) &gt; 0), ROW(J$3:INDEX(J:J,$F$1))), MIN($H$303, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", J$3:INDEX(J:J,$F$1), "&gt;0")))))), 0)</f>
         <v>152</v>
       </c>
-      <c r="K203" cm="1">
-        <f t="array" ref="K203">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:K$200, ($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0) * (ROW(K$3:K$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (K$3:K$200 &gt; 0), ROW(K$3:K$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", K$3:K$200, "&gt;0")))))), 0)</f>
+      <c r="K303" cm="1">
+        <f t="array" ref="K303">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:INDEX(K:K,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (K$3:INDEX(K:K,$F$1) &gt; 0) * (ROW(K$3:INDEX(K:K,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (K$3:INDEX(K:K,$F$1) &gt; 0), ROW(K$3:INDEX(K:K,$F$1))), MIN($H$303, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", K$3:INDEX(K:K,$F$1), "&gt;0")))))), 0)</f>
         <v>877</v>
       </c>
-      <c r="L203" cm="1">
-        <f t="array" ref="L203">IFERROR(SUM(_xlfn._xlws.FILTER(L$3:L$200, ($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0) * (ROW(L$3:L$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (L$3:L$200 &gt; 0), ROW(L$3:L$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", L$3:L$200, "&gt;0")))))), 0)</f>
+      <c r="L303" cm="1">
+        <f t="array" ref="L303">IFERROR(SUM(_xlfn._xlws.FILTER(L$3:INDEX(L:L,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (L$3:INDEX(L:L,$F$1) &gt; 0) * (ROW(L$3:INDEX(L:L,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (L$3:INDEX(L:L,$F$1) &gt; 0), ROW(L$3:INDEX(L:L,$F$1))), MIN($H$303, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", L$3:INDEX(L:L,$F$1), "&gt;0")))))), 0)</f>
         <v>829</v>
       </c>
-      <c r="M203" cm="1">
-        <f t="array" ref="M203">IFERROR(SUM(_xlfn._xlws.FILTER(M$3:M$200, ($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0) * (ROW(M$3:M$200) &gt;= LARGE(IF(($G$3:$G$200&lt;&gt;"") * (M$3:M$200 &gt; 0), ROW(M$3:M$200)), MIN($H$203, COUNTIFS($G$3:$G$200, "&lt;&gt;", M$3:M$200, "&gt;0")))))), 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I204" t="str">
+      <c r="M303" cm="1">
+        <f t="array" ref="M303">IFERROR(SUM(_xlfn._xlws.FILTER(M$3:INDEX(M:M,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (M$3:INDEX(M:M,$F$1) &gt; 0) * (ROW(M$3:INDEX(M:M,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (M$3:INDEX(M:M,$F$1) &gt; 0), ROW(M$3:INDEX(M:M,$F$1))), MIN($H$303, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", M$3:INDEX(M:M,$F$1), "&gt;0")))))), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I304" t="str">
         <f>I$2</f>
         <v>adalfarus</v>
       </c>
-      <c r="J204" t="str">
-        <f t="shared" ref="J204:M204" si="5">J$2</f>
+      <c r="J304" t="str">
+        <f t="shared" ref="J204:M304" si="7">J$2</f>
         <v>Giesbrt</v>
       </c>
-      <c r="K204" t="str">
-        <f t="shared" si="5"/>
+      <c r="K304" t="str">
+        <f t="shared" si="7"/>
         <v>Fa4953</v>
       </c>
-      <c r="L204" t="str">
-        <f t="shared" si="5"/>
+      <c r="L304" t="str">
+        <f t="shared" si="7"/>
         <v>TheCodeJak</v>
       </c>
-      <c r="M204" t="str">
-        <f t="shared" si="5"/>
+      <c r="M304" t="str">
+        <f t="shared" si="7"/>
         <v>MNcode24</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G205" t="s">
+    <row r="305" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G305" t="s">
         <v>164</v>
       </c>
-      <c r="I205">
-        <f>COUNTIF($G$3:$G$200, I$2)</f>
+      <c r="I305">
+        <f>COUNTIF($G$3:INDEX($G:$G,$F$1), I$2)</f>
         <v>59</v>
       </c>
-      <c r="J205">
-        <f>COUNTIF($G$3:$G$200, J$2)</f>
+      <c r="J305">
+        <f>COUNTIF($G$3:INDEX($G:$G,$F$1), J$2)</f>
         <v>98</v>
       </c>
-      <c r="K205">
-        <f>COUNTIF($G$3:$G$200, K$2)</f>
+      <c r="K305">
+        <f>COUNTIF($G$3:INDEX($G:$G,$F$1), K$2)</f>
         <v>12</v>
       </c>
-      <c r="L205">
-        <f>COUNTIF($G$3:$G$200, L$2)</f>
+      <c r="L305">
+        <f>COUNTIF($G$3:INDEX($G:$G,$F$1), L$2)</f>
         <v>7</v>
       </c>
-      <c r="M205">
-        <f>COUNTIF($G$3:$G$200, M$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G206" t="s">
+      <c r="M305">
+        <f>COUNTIF($G$3:INDEX($G:$G,$F$1), M$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G306" t="s">
         <v>165</v>
       </c>
-      <c r="I206">
-        <f>IF(COUNTIF($G$3:$G$200, I$2) &gt; 0, AVERAGEIF($G$3:$G$200, I$2, $E$3:$E$200), 0)</f>
+      <c r="I306">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
         <v>1.4067796610169492</v>
       </c>
-      <c r="J206">
-        <f>IF(COUNTIF($G$3:$G$200, J$2) &gt; 0, AVERAGEIF($G$3:$G$200, J$2, $E$3:$E$200), 0)</f>
+      <c r="J306">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
         <v>1.4072164948453609</v>
       </c>
-      <c r="K206">
-        <f>IF(COUNTIF($G$3:$G$200, K$2) &gt; 0, AVERAGEIF($G$3:$G$200, K$2, $E$3:$E$200), 0)</f>
+      <c r="K306">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), K$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), K$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
         <v>1.75</v>
       </c>
-      <c r="L206">
-        <f>IF(COUNTIF($G$3:$G$200, L$2) &gt; 0, AVERAGEIF($G$3:$G$200, L$2, $E$3:$E$200), 0)</f>
+      <c r="L306">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), L$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), L$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
         <v>1.2857142857142858</v>
       </c>
-      <c r="M206">
+      <c r="M306">
         <f>IF(COUNTIF($G$3:$G$200, M$2) &gt; 0, AVERAGEIF($G$3:$G$200, M$2, $E$3:$E$200), 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G207" t="s">
+    <row r="307" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G307" t="s">
         <v>166</v>
       </c>
-      <c r="I207">
-        <f>IF(COUNTIF($G$3:$G$200, I$2) &gt; 0, AVERAGEIF($G$3:$G$200, I$2, $D$3:$D$200), 0)</f>
+      <c r="I307">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
         <v>41.813559322033896</v>
       </c>
-      <c r="J207">
-        <f>IF(COUNTIF($G$3:$G$200, J$2) &gt; 0, AVERAGEIF($G$3:$G$200, J$2, $D$3:$D$200), 0)</f>
+      <c r="J307">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
         <v>20.226804123711339</v>
       </c>
-      <c r="K207">
-        <f>IF(COUNTIF($G$3:$G$200, K$2) &gt; 0, AVERAGEIF($G$3:$G$200, K$2, $D$3:$D$200), 0)</f>
+      <c r="K307">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), K$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), K$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
         <v>36.166666666666664</v>
       </c>
-      <c r="L207">
-        <f>IF(COUNTIF($G$3:$G$200, L$2) &gt; 0, AVERAGEIF($G$3:$G$200, L$2, $D$3:$D$200), 0)</f>
+      <c r="L307">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), L$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), L$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
         <v>77.428571428571431</v>
       </c>
-      <c r="M207">
-        <f>IF(COUNTIF($G$3:$G$200, M$2) &gt; 0, AVERAGEIF($G$3:$G$200, M$2, $D$3:$D$200), 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G208" t="s">
+      <c r="M307">
+        <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), M$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), M$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G308" t="s">
         <v>167</v>
       </c>
-      <c r="I208">
-        <f>ROUND(I$205*I$206*I$207, 0)</f>
+      <c r="I308">
+        <f>ROUND(I$305*I$306*I$307, 0)</f>
         <v>3471</v>
       </c>
-      <c r="J208">
-        <f>ROUND(J$205*J$206*J$207, 0)</f>
+      <c r="J308">
+        <f>ROUND(J$305*J$306*J$307, 0)</f>
         <v>2789</v>
       </c>
-      <c r="K208">
-        <f>ROUND(K$205*K$206*K$207, 0)</f>
+      <c r="K308">
+        <f>ROUND(K$305*K$306*K$307, 0)</f>
         <v>760</v>
       </c>
-      <c r="L208">
-        <f>ROUND(L$205*L$206*L$207, 0)</f>
+      <c r="L308">
+        <f>ROUND(L$305*L$306*L$307, 0)</f>
         <v>697</v>
       </c>
-      <c r="M208">
-        <f>ROUND(M$205*M$206*M$207, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G210" t="s">
+      <c r="M308">
+        <f>ROUND(M$305*M$306*M$307, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G310" t="s">
         <v>168</v>
       </c>
-      <c r="I210" t="str">
+      <c r="I310" t="str">
         <f>I$2</f>
         <v>adalfarus</v>
       </c>
-      <c r="J210" t="str">
-        <f t="shared" ref="J210:M210" si="6">J$2</f>
+      <c r="J310" t="str">
+        <f t="shared" ref="J210:M310" si="8">J$2</f>
         <v>Giesbrt</v>
       </c>
-      <c r="K210" t="str">
-        <f t="shared" si="6"/>
+      <c r="K310" t="str">
+        <f t="shared" si="8"/>
         <v>Fa4953</v>
       </c>
-      <c r="L210" t="str">
-        <f t="shared" si="6"/>
+      <c r="L310" t="str">
+        <f t="shared" si="8"/>
         <v>TheCodeJak</v>
       </c>
-      <c r="M210" t="str">
-        <f t="shared" si="6"/>
+      <c r="M310" t="str">
+        <f t="shared" si="8"/>
         <v>MNcode24</v>
       </c>
     </row>
-    <row r="211" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G211" t="str" cm="1">
-        <f t="array" ref="G211:G223">_xlfn._xlws.FILTER(_xlfn.UNIQUE(C3:C200), _xlfn.UNIQUE(C3:C200)&lt;&gt;0)</f>
+    <row r="311" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G311" t="str" cm="1">
+        <f t="array" ref="G311:G323">_xlfn._xlws.FILTER(_xlfn.UNIQUE(C3:C200), _xlfn.UNIQUE(C3:C200)&lt;&gt;0)</f>
         <v>everything</v>
       </c>
-      <c r="I211">
-        <f t="shared" ref="I211:L222" si="7">COUNTIFS($G$3:$G$200, I$210, $C$3:$C$200, $G211)</f>
+      <c r="I311">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G311)</f>
         <v>12</v>
       </c>
-      <c r="J211">
-        <f t="shared" si="7"/>
+      <c r="J311">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G311)</f>
         <v>23</v>
       </c>
-      <c r="K211">
-        <f t="shared" si="7"/>
+      <c r="K311">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G311)</f>
         <v>8</v>
       </c>
-      <c r="L211">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M211">
-        <f>COUNTIFS(C3:C200, G211, G3:G200, M210)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G212" t="str">
+      <c r="L311">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G311)</f>
+        <v>0</v>
+      </c>
+      <c r="M311">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G311)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G312" t="str">
         <v>changes</v>
       </c>
-      <c r="I212">
-        <f t="shared" si="7"/>
+      <c r="I312">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G312)</f>
         <v>22</v>
       </c>
-      <c r="J212">
-        <f t="shared" si="7"/>
+      <c r="J312">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G312)</f>
         <v>32</v>
       </c>
-      <c r="K212">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L212">
-        <f t="shared" si="7"/>
+      <c r="K312">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G312)</f>
+        <v>0</v>
+      </c>
+      <c r="L312">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G312)</f>
         <v>4</v>
       </c>
-      <c r="M212">
-        <f t="shared" ref="M212:M222" si="8">COUNTIFS($G$3:$G$200, M$210, $C$3:$C$200, $G212)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G213" t="str">
+      <c r="M312">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G312)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G313" t="str">
         <v>new cls</v>
       </c>
-      <c r="I213">
-        <f t="shared" si="7"/>
+      <c r="I313">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G313)</f>
         <v>1</v>
       </c>
-      <c r="J213">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K213">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L213">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M213">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G214" t="str">
+      <c r="J313">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G313)</f>
+        <v>0</v>
+      </c>
+      <c r="K313">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G313)</f>
+        <v>0</v>
+      </c>
+      <c r="L313">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G313)</f>
+        <v>0</v>
+      </c>
+      <c r="M313">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G313)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G314" t="str">
         <v>docs</v>
       </c>
-      <c r="I214">
-        <f t="shared" si="7"/>
+      <c r="I314">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G314)</f>
         <v>1</v>
       </c>
-      <c r="J214">
-        <f t="shared" si="7"/>
+      <c r="J314">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G314)</f>
         <v>13</v>
       </c>
-      <c r="K214">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L214">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M214">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G215" t="str">
+      <c r="K314">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G314)</f>
+        <v>0</v>
+      </c>
+      <c r="L314">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G314)</f>
+        <v>0</v>
+      </c>
+      <c r="M314">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G314)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G315" t="str">
         <v>change docs</v>
       </c>
-      <c r="I215">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J215">
-        <f t="shared" si="7"/>
+      <c r="I315">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G315)</f>
+        <v>0</v>
+      </c>
+      <c r="J315">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G315)</f>
         <v>3</v>
       </c>
-      <c r="K215">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L215">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M215">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G216" t="str">
+      <c r="K315">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G315)</f>
+        <v>0</v>
+      </c>
+      <c r="L315">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G315)</f>
+        <v>0</v>
+      </c>
+      <c r="M315">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G315)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G316" t="str">
         <v>remove</v>
       </c>
-      <c r="I216">
-        <f t="shared" si="7"/>
+      <c r="I316">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G316)</f>
         <v>1</v>
       </c>
-      <c r="J216">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K216">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L216">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M216">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G217" t="str">
+      <c r="J316">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G316)</f>
+        <v>0</v>
+      </c>
+      <c r="K316">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G316)</f>
+        <v>0</v>
+      </c>
+      <c r="L316">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G316)</f>
+        <v>0</v>
+      </c>
+      <c r="M316">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G316)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G317" t="str">
         <v>created</v>
       </c>
-      <c r="I217">
-        <f t="shared" si="7"/>
+      <c r="I317">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G317)</f>
         <v>1</v>
       </c>
-      <c r="J217">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K217">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L217">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M217">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G218" t="str">
+      <c r="J317">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G317)</f>
+        <v>0</v>
+      </c>
+      <c r="K317">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G317)</f>
+        <v>0</v>
+      </c>
+      <c r="L317">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G317)</f>
+        <v>0</v>
+      </c>
+      <c r="M317">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G317)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G318" t="str">
         <v>smaller updates</v>
       </c>
-      <c r="I218">
-        <f t="shared" si="7"/>
+      <c r="I318">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G318)</f>
         <v>1</v>
       </c>
-      <c r="J218">
-        <f t="shared" si="7"/>
+      <c r="J318">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G318)</f>
         <v>1</v>
       </c>
-      <c r="K218">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L218">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M218">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G219" t="str">
+      <c r="K318">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G318)</f>
+        <v>0</v>
+      </c>
+      <c r="L318">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G318)</f>
+        <v>0</v>
+      </c>
+      <c r="M318">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G318)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G319" t="str">
         <v>added</v>
       </c>
-      <c r="I219">
-        <f t="shared" si="7"/>
+      <c r="I319">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G319)</f>
         <v>19</v>
       </c>
-      <c r="J219">
-        <f t="shared" si="7"/>
+      <c r="J319">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G319)</f>
         <v>24</v>
       </c>
-      <c r="K219">
-        <f t="shared" si="7"/>
+      <c r="K319">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G319)</f>
         <v>3</v>
       </c>
-      <c r="L219">
-        <f t="shared" si="7"/>
+      <c r="L319">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G319)</f>
         <v>3</v>
       </c>
-      <c r="M219">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G220" t="str">
+      <c r="M319">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G319)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G320" t="str">
         <v>setter</v>
       </c>
-      <c r="I220">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J220">
-        <f t="shared" si="7"/>
+      <c r="I320">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G320)</f>
+        <v>0</v>
+      </c>
+      <c r="J320">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G320)</f>
         <v>1</v>
       </c>
-      <c r="K220">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L220">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M220">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G221" t="str">
+      <c r="K320">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G320)</f>
+        <v>0</v>
+      </c>
+      <c r="L320">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G320)</f>
+        <v>0</v>
+      </c>
+      <c r="M320">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G320)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G321" t="str">
         <v>moved</v>
       </c>
-      <c r="I221">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J221">
-        <f t="shared" si="7"/>
+      <c r="I321">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G321)</f>
+        <v>0</v>
+      </c>
+      <c r="J321">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G321)</f>
         <v>1</v>
       </c>
-      <c r="K221">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L221">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M221">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G222" t="str">
+      <c r="K321">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G321)</f>
+        <v>0</v>
+      </c>
+      <c r="L321">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G321)</f>
+        <v>0</v>
+      </c>
+      <c r="M321">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G321)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G322" t="str">
         <v>fixes</v>
       </c>
-      <c r="I222">
-        <f t="shared" si="7"/>
+      <c r="I322">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$310, $C$3:INDEX($C:$C,$F$1), $G322)</f>
         <v>1</v>
       </c>
-      <c r="J222">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K222">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L222">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M222">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G223" t="str">
+      <c r="J322">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$310, $C$3:INDEX($C:$C,$F$1), $G322)</f>
+        <v>0</v>
+      </c>
+      <c r="K322">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$310, $C$3:INDEX($C:$C,$F$1), $G322)</f>
+        <v>0</v>
+      </c>
+      <c r="L322">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$310, $C$3:INDEX($C:$C,$F$1), $G322)</f>
+        <v>0</v>
+      </c>
+      <c r="M322">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$310, $C$3:INDEX($C:$C,$F$1), $G322)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G323" t="str">
         <v>one line</v>
       </c>
     </row>
-    <row r="225" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G225" t="s">
+    <row r="325" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G325" t="s">
         <v>169</v>
       </c>
-      <c r="I225" t="str">
-        <f t="shared" ref="I225:M225" si="9">I$2</f>
+      <c r="I325" t="str">
+        <f t="shared" ref="I225:M325" si="9">I$2</f>
         <v>adalfarus</v>
       </c>
-      <c r="J225" t="str">
+      <c r="J325" t="str">
         <f t="shared" si="9"/>
         <v>Giesbrt</v>
       </c>
-      <c r="K225" t="str">
+      <c r="K325" t="str">
         <f t="shared" si="9"/>
         <v>Fa4953</v>
       </c>
-      <c r="L225" t="str">
+      <c r="L325" t="str">
         <f t="shared" si="9"/>
         <v>TheCodeJak</v>
       </c>
-      <c r="M225" t="str">
+      <c r="M325" t="str">
         <f t="shared" si="9"/>
         <v>MNcode24</v>
       </c>
     </row>
-    <row r="226" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G226" t="str" cm="1">
-        <f t="array" ref="G226:G232">_xlfn._xlws.FILTER(_xlfn.UNIQUE(F3:F200), _xlfn.UNIQUE(F3:F200)&lt;&gt;0)</f>
+    <row r="326" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G326" t="str" cm="1">
+        <f t="array" ref="G326:G332">_xlfn._xlws.FILTER(_xlfn.UNIQUE(F3:F200), _xlfn.UNIQUE(F3:F200)&lt;&gt;0)</f>
         <v>none</v>
       </c>
-      <c r="I226">
-        <f t="shared" ref="I226:M232" si="10">COUNTIFS($G$3:$G$200, I$225, $F$3:$F$200, $G226)</f>
+      <c r="I326">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G326)</f>
         <v>47</v>
       </c>
-      <c r="J226">
+      <c r="J326">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G326)</f>
+        <v>58</v>
+      </c>
+      <c r="K326">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G326)</f>
+        <v>2</v>
+      </c>
+      <c r="L326">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G326)</f>
+        <v>7</v>
+      </c>
+      <c r="M326">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G326)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G327" t="str">
+        <v>comments 5%</v>
+      </c>
+      <c r="I327">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G327)</f>
+        <v>2</v>
+      </c>
+      <c r="J327">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G327)</f>
+        <v>0</v>
+      </c>
+      <c r="K327">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G327)</f>
+        <v>0</v>
+      </c>
+      <c r="L327">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G327)</f>
+        <v>0</v>
+      </c>
+      <c r="M327">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G327)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G328" t="str">
+        <v>inline 100%</v>
+      </c>
+      <c r="I328">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G328)</f>
+        <v>5</v>
+      </c>
+      <c r="J328">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G328)</f>
+        <v>38</v>
+      </c>
+      <c r="K328">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G328)</f>
+        <v>10</v>
+      </c>
+      <c r="L328">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G328)</f>
+        <v>0</v>
+      </c>
+      <c r="M328">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G328)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G329" t="str">
+        <v>inline 5%</v>
+      </c>
+      <c r="I329">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G329)</f>
+        <v>3</v>
+      </c>
+      <c r="J329">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G329)</f>
+        <v>0</v>
+      </c>
+      <c r="K329">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G329)</f>
+        <v>0</v>
+      </c>
+      <c r="L329">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G329)</f>
+        <v>0</v>
+      </c>
+      <c r="M329">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G329)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G330" t="str">
+        <v>comments 100%</v>
+      </c>
+      <c r="I330">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G330)</f>
+        <v>1</v>
+      </c>
+      <c r="J330">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G330)</f>
+        <v>0</v>
+      </c>
+      <c r="K330">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G330)</f>
+        <v>0</v>
+      </c>
+      <c r="L330">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G330)</f>
+        <v>0</v>
+      </c>
+      <c r="M330">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G330)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G331" t="str">
+        <v>inline 50%</v>
+      </c>
+      <c r="I331">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G331)</f>
+        <v>0</v>
+      </c>
+      <c r="J331">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G331)</f>
+        <v>2</v>
+      </c>
+      <c r="K331">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G331)</f>
+        <v>0</v>
+      </c>
+      <c r="L331">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G331)</f>
+        <v>0</v>
+      </c>
+      <c r="M331">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G331)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G332" t="str">
+        <v>in md 100%</v>
+      </c>
+      <c r="I332">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$325, $F$3:INDEX($F:$F,$F$1), $G332)</f>
+        <v>1</v>
+      </c>
+      <c r="J332">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$325, $F$3:INDEX($F:$F,$F$1), $G332)</f>
+        <v>0</v>
+      </c>
+      <c r="K332">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$325, $F$3:INDEX($F:$F,$F$1), $G332)</f>
+        <v>0</v>
+      </c>
+      <c r="L332">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$325, $F$3:INDEX($F:$F,$F$1), $G332)</f>
+        <v>0</v>
+      </c>
+      <c r="M332">
+        <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$325, $F$3:INDEX($F:$F,$F$1), $G332)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="I335" t="str">
+        <f t="shared" ref="I238:M335" si="10">I$2</f>
+        <v>adalfarus</v>
+      </c>
+      <c r="J335" t="str">
         <f t="shared" si="10"/>
-        <v>58</v>
-      </c>
-      <c r="K226">
+        <v>Giesbrt</v>
+      </c>
+      <c r="K335" t="str">
         <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="L226">
+        <v>Fa4953</v>
+      </c>
+      <c r="L335" t="str">
         <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="M226">
+        <v>TheCodeJak</v>
+      </c>
+      <c r="M335" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G227" t="str">
-        <v>comments 5%</v>
-      </c>
-      <c r="I227">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="J227">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K227">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L227">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M227">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G228" t="str">
-        <v>inline 100%</v>
-      </c>
-      <c r="I228">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="J228">
-        <f t="shared" si="10"/>
-        <v>38</v>
-      </c>
-      <c r="K228">
-        <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="L228">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M228">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G229" t="str">
-        <v>inline 5%</v>
-      </c>
-      <c r="I229">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="J229">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K229">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L229">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M229">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G230" t="str">
-        <v>comments 100%</v>
-      </c>
-      <c r="I230">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="J230">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K230">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L230">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M230">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G231" t="str">
-        <v>inline 50%</v>
-      </c>
-      <c r="I231">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J231">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="K231">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L231">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M231">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G232" t="str">
-        <v>in md 100%</v>
-      </c>
-      <c r="I232">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="J232">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K232">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L232">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M232">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="I238" t="str">
-        <f t="shared" ref="I238:M238" si="11">I$2</f>
-        <v>adalfarus</v>
-      </c>
-      <c r="J238" t="str">
-        <f t="shared" si="11"/>
-        <v>Giesbrt</v>
-      </c>
-      <c r="K238" t="str">
-        <f t="shared" si="11"/>
-        <v>Fa4953</v>
-      </c>
-      <c r="L238" t="str">
-        <f t="shared" si="11"/>
-        <v>TheCodeJak</v>
-      </c>
-      <c r="M238" t="str">
-        <f t="shared" si="11"/>
         <v>MNcode24</v>
       </c>
     </row>
-    <row r="239" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G239" t="s">
+    <row r="336" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G336" t="s">
         <v>233</v>
       </c>
-      <c r="H239">
-        <f>SUM(I201:M201)</f>
+      <c r="H336">
+        <f>SUM(I301:M301)</f>
         <v>8754</v>
       </c>
-      <c r="I239" s="16">
-        <f>I201/$H239</f>
+      <c r="I336" s="16">
+        <f>I301/$H336</f>
         <v>0.43791409641306833</v>
       </c>
-      <c r="J239" s="16">
-        <f t="shared" ref="J239:M239" si="12">J201/$H239</f>
+      <c r="J336" s="16">
+        <f>J301/$H336</f>
         <v>0.36720356408498972</v>
       </c>
-      <c r="K239" s="16">
-        <f t="shared" si="12"/>
+      <c r="K336" s="16">
+        <f>K301/$H336</f>
         <v>0.10018277358921636</v>
       </c>
-      <c r="L239" s="16">
-        <f t="shared" si="12"/>
+      <c r="L336" s="16">
+        <f>L301/$H336</f>
         <v>9.4699565912725617E-2</v>
       </c>
-      <c r="M239" s="16">
-        <f t="shared" si="12"/>
+      <c r="M336" s="16">
+        <f>M301/$H336</f>
         <v>0</v>
       </c>
     </row>
@@ -19815,7 +22160,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Added latest commit to housekeeping
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/CommitTable.xlsx
+++ b/meta/dudpy-planning/CommitTable.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011938C6-2A18-476C-923C-6BDE98CF1B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDAF35A-E97C-422E-99AB-7AD5EC5189DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="324">
   <si>
     <t>Datei</t>
   </si>
@@ -1060,6 +1060,9 @@
   </si>
   <si>
     <t>Perfected zooming and ...</t>
+  </si>
+  <si>
+    <t>Cleaned up _grids.py a...</t>
   </si>
 </sst>
 </file>
@@ -2056,7 +2059,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -2988,7 +2991,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -3711,7 +3714,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>108</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>146</c:v>
@@ -3788,7 +3791,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2611111111111111</c:v>
+                  <c:v>1.2495412844036695</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.348965517241379</c:v>
@@ -3865,7 +3868,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>28.574074074074073</c:v>
+                  <c:v>28.311926605504588</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19.627586206896552</c:v>
@@ -4556,7 +4559,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3892</c:v>
+                  <c:v>3856</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3866</c:v>
@@ -10899,8 +10902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N536"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I501" sqref="I501"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H327" sqref="H327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24289,7 +24292,7 @@
       </c>
       <c r="H302" s="8"/>
       <c r="I302">
-        <f t="shared" ref="I302:M365" si="16">MAX(0, IF($G302=I$2, $D302*$E302, 0))</f>
+        <f t="shared" ref="I302:M352" si="16">MAX(0, IF($G302=I$2, $D302*$E302, 0))</f>
         <v>8</v>
       </c>
       <c r="J302">
@@ -25377,7 +25380,27 @@
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B327" s="7"/>
+      <c r="A327" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B327" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C327" t="s">
+        <v>173</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="F327" t="s">
+        <v>24</v>
+      </c>
+      <c r="G327" t="s">
+        <v>15</v>
+      </c>
       <c r="H327" s="8"/>
       <c r="I327">
         <f t="shared" si="16"/>
@@ -26004,7 +26027,7 @@
       <c r="B353" s="7"/>
       <c r="H353" s="8"/>
       <c r="I353">
-        <f t="shared" ref="I353:M416" si="17">MAX(0, IF($G353=I$2, $D353*$E353, 0))</f>
+        <f t="shared" ref="I353:M403" si="17">MAX(0, IF($G353=I$2, $D353*$E353, 0))</f>
         <v>0</v>
       </c>
       <c r="J353">
@@ -27228,7 +27251,7 @@
       <c r="B404" s="7"/>
       <c r="H404" s="8"/>
       <c r="I404">
-        <f t="shared" ref="I404:M467" si="18">MAX(0, IF($G404=I$2, $D404*$E404, 0))</f>
+        <f t="shared" ref="I404:M454" si="18">MAX(0, IF($G404=I$2, $D404*$E404, 0))</f>
         <v>0</v>
       </c>
       <c r="J404">
@@ -29660,7 +29683,7 @@
         <v>adalfarus</v>
       </c>
       <c r="J504" t="str">
-        <f t="shared" ref="J304:M504" si="20">J$2</f>
+        <f t="shared" ref="J504:M504" si="20">J$2</f>
         <v>Giesbrt</v>
       </c>
       <c r="K504" t="str">
@@ -29682,7 +29705,7 @@
       </c>
       <c r="I505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), I$2)</f>
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), J$2)</f>
@@ -29707,7 +29730,7 @@
       </c>
       <c r="I506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
-        <v>1.2611111111111111</v>
+        <v>1.2495412844036695</v>
       </c>
       <c r="J506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
@@ -29732,7 +29755,7 @@
       </c>
       <c r="I507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
-        <v>28.574074074074073</v>
+        <v>28.311926605504588</v>
       </c>
       <c r="J507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
@@ -29757,7 +29780,7 @@
       </c>
       <c r="I508">
         <f>ROUND(I$505*I$506*I$507, 0)</f>
-        <v>3892</v>
+        <v>3856</v>
       </c>
       <c r="J508">
         <f>ROUND(J$505*J$506*J$507, 0)</f>
@@ -29785,7 +29808,7 @@
         <v>adalfarus</v>
       </c>
       <c r="J510" t="str">
-        <f t="shared" ref="J310:M510" si="21">J$2</f>
+        <f t="shared" ref="J510:M510" si="21">J$2</f>
         <v>Giesbrt</v>
       </c>
       <c r="K510" t="str">
@@ -29933,7 +29956,7 @@
       </c>
       <c r="I516">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$510, $C$3:INDEX($C:$C,$F$1), $G516)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J516">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$510, $C$3:INDEX($C:$C,$F$1), $G516)</f>
@@ -30112,7 +30135,7 @@
         <v>169</v>
       </c>
       <c r="I525" t="str">
-        <f t="shared" ref="I325:M525" si="22">I$2</f>
+        <f t="shared" ref="I525:M525" si="22">I$2</f>
         <v>adalfarus</v>
       </c>
       <c r="J525" t="str">
@@ -30214,7 +30237,7 @@
       </c>
       <c r="I529">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$525, $F$3:INDEX($F:$F,$F$1), $G529)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J529">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$525, $F$3:INDEX($F:$F,$F$1), $G529)</f>
@@ -30310,7 +30333,7 @@
     </row>
     <row r="535" spans="7:13" x14ac:dyDescent="0.25">
       <c r="I535" t="str">
-        <f t="shared" ref="I335:M535" si="23">I$2</f>
+        <f t="shared" ref="I535:M535" si="23">I$2</f>
         <v>adalfarus</v>
       </c>
       <c r="J535" t="str">
@@ -30510,10 +30533,11 @@
     <hyperlink ref="A323" r:id="rId144" xr:uid="{9995317C-A983-44BD-91A4-A9D1CAF17AD0}"/>
     <hyperlink ref="A324" r:id="rId145" xr:uid="{69E6B5BE-C75F-4DCF-9F04-DE748577573F}"/>
     <hyperlink ref="A326" r:id="rId146" xr:uid="{767A3ED2-94F0-472F-BAC7-6AD204629CC8}"/>
+    <hyperlink ref="A327" r:id="rId147" xr:uid="{89D0DE87-BFB9-4160-8911-7E9A1AE7C1D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId147"/>
-  <drawing r:id="rId148"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId148"/>
+  <drawing r:id="rId149"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed None error and updated Housekeeping a bit
</commit_message>
<xml_diff>
--- a/meta/dudpy-planning/CommitTable.xlsx
+++ b/meta/dudpy-planning/CommitTable.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B307D74-25F2-42D3-8C64-E0884262E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6073AF8-16C1-482F-B6BE-44A499B79A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tätigkeitsdokumentation" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="341">
   <si>
     <t>Datei</t>
   </si>
@@ -1063,6 +1063,57 @@
   </si>
   <si>
     <t>Cleaned up _grids.py a...</t>
+  </si>
+  <si>
+    <t>Updated release version ...</t>
+  </si>
+  <si>
+    <t>reworked BaseStruct.d...</t>
+  </si>
+  <si>
+    <t>meta\BaseStruct.drawio</t>
+  </si>
+  <si>
+    <t>First implementation ...</t>
+  </si>
+  <si>
+    <t>pyside.py</t>
+  </si>
+  <si>
+    <t>Improved pyside.py ...</t>
+  </si>
+  <si>
+    <t>New Styles</t>
+  </si>
+  <si>
+    <t>Implemented set_settings</t>
+  </si>
+  <si>
+    <t>New Settings Button</t>
+  </si>
+  <si>
+    <t>Update extension...</t>
+  </si>
+  <si>
+    <t>undo changes extens...</t>
+  </si>
+  <si>
+    <t>Fixed app not starting</t>
+  </si>
+  <si>
+    <t>Changes to serializer</t>
+  </si>
+  <si>
+    <t>added upload method</t>
+  </si>
+  <si>
+    <t>updated logic</t>
+  </si>
+  <si>
+    <t>Implemented abstract method</t>
+  </si>
+  <si>
+    <t>GUI changes to menu ...</t>
   </si>
 </sst>
 </file>
@@ -1312,9 +1363,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1332,7 +1383,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1805,19 +1856,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4695.7999999999993</c:v>
+                  <c:v>4890.7999999999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4702.3</c:v>
+                  <c:v>5281.9000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1403</c:v>
+                  <c:v>1552.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3792.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1895,7 +1946,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2043,10 +2094,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -2067,7 +2118,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2162,10 +2213,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2186,7 +2237,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -2296,7 +2347,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2305,7 +2356,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2519,7 +2570,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2543,7 +2594,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2783,7 +2834,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2981,7 +3032,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -3070,13 +3121,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -3159,7 +3210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3337,7 +3388,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3586,7 +3637,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3713,19 +3764,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3790,13 +3841,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2495412844036695</c:v>
+                  <c:v>1.2427350427350425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3524137931034481</c:v>
+                  <c:v>1.399354838709677</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>1.4119999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.555102040816327</c:v>
@@ -3867,19 +3918,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>28.311926605504588</c:v>
+                  <c:v>27.743589743589745</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.627586206896552</c:v>
+                  <c:v>20.677419354838708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.85</c:v>
+                  <c:v>28.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>46.673469387755105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4109,7 +4160,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4558,13 +4609,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3856</c:v>
+                  <c:v>4034</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3876</c:v>
+                  <c:v>4514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>986</c:v>
+                  <c:v>1001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3557</c:v>
@@ -4648,7 +4699,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4925,16 +4976,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>127.2</c:v>
+                  <c:v>72.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>194</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -5057,7 +5108,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5334,19 +5385,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>316</c:v>
+                  <c:v>430.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>680</c:v>
+                  <c:v>808.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>982</c:v>
+                  <c:v>794.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1196.0999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5466,7 +5517,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5726,19 +5777,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.32177118736980592</c:v>
+                  <c:v>0.31156950558376273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32221658809341086</c:v>
+                  <c:v>0.33648461837386051</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6138033110404572E-2</c:v>
+                  <c:v>9.8876876915138259E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25987419142637869</c:v>
+                  <c:v>0.24160205895281353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.14669401744249E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10579,9 +10630,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -10619,9 +10670,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10654,9 +10705,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10689,9 +10757,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -10867,11 +10952,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M536"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A494" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K503" sqref="K503"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C353" sqref="C353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
@@ -25388,11 +25473,31 @@
       </c>
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B328" s="7"/>
+      <c r="A328" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B328" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C328" t="s">
+        <v>149</v>
+      </c>
+      <c r="D328">
+        <v>15</v>
+      </c>
+      <c r="E328">
+        <v>3</v>
+      </c>
+      <c r="F328" t="s">
+        <v>18</v>
+      </c>
+      <c r="G328" t="s">
+        <v>15</v>
+      </c>
       <c r="H328" s="8"/>
       <c r="I328">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J328">
         <f t="shared" si="16"/>
@@ -25412,7 +25517,27 @@
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B329" s="7"/>
+      <c r="A329" t="s">
+        <v>214</v>
+      </c>
+      <c r="B329" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C329" t="s">
+        <v>27</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329">
+        <v>0</v>
+      </c>
+      <c r="F329" t="s">
+        <v>18</v>
+      </c>
+      <c r="G329" t="s">
+        <v>15</v>
+      </c>
       <c r="H329" s="8"/>
       <c r="I329">
         <f t="shared" si="16"/>
@@ -25436,7 +25561,27 @@
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B330" s="7"/>
+      <c r="A330" t="s">
+        <v>128</v>
+      </c>
+      <c r="B330" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C330" t="s">
+        <v>27</v>
+      </c>
+      <c r="D330">
+        <v>1</v>
+      </c>
+      <c r="E330">
+        <v>1</v>
+      </c>
+      <c r="F330" t="s">
+        <v>18</v>
+      </c>
+      <c r="G330" t="s">
+        <v>34</v>
+      </c>
       <c r="H330" s="8"/>
       <c r="I330">
         <f t="shared" si="16"/>
@@ -25444,7 +25589,7 @@
       </c>
       <c r="J330">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K330">
         <f t="shared" si="16"/>
@@ -25460,7 +25605,27 @@
       </c>
     </row>
     <row r="331" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B331" s="7"/>
+      <c r="A331" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B331" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C331" t="s">
+        <v>28</v>
+      </c>
+      <c r="D331">
+        <v>80</v>
+      </c>
+      <c r="E331">
+        <v>0.6</v>
+      </c>
+      <c r="F331" t="s">
+        <v>18</v>
+      </c>
+      <c r="G331" t="s">
+        <v>34</v>
+      </c>
       <c r="H331" s="8"/>
       <c r="I331">
         <f t="shared" si="16"/>
@@ -25468,7 +25633,7 @@
       </c>
       <c r="J331">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="K331">
         <f t="shared" si="16"/>
@@ -25484,7 +25649,28 @@
       </c>
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B332" s="7"/>
+      <c r="A332" t="s">
+        <v>128</v>
+      </c>
+      <c r="B332" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C332" t="s">
+        <v>149</v>
+      </c>
+      <c r="D332">
+        <f>2+31</f>
+        <v>33</v>
+      </c>
+      <c r="E332">
+        <v>1.2</v>
+      </c>
+      <c r="F332" t="s">
+        <v>19</v>
+      </c>
+      <c r="G332" t="s">
+        <v>34</v>
+      </c>
       <c r="H332" s="8"/>
       <c r="I332">
         <f t="shared" si="16"/>
@@ -25492,7 +25678,7 @@
       </c>
       <c r="J332">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>39.6</v>
       </c>
       <c r="K332">
         <f t="shared" si="16"/>
@@ -25508,7 +25694,27 @@
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B333" s="7"/>
+      <c r="A333" t="s">
+        <v>128</v>
+      </c>
+      <c r="B333" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C333" t="s">
+        <v>27</v>
+      </c>
+      <c r="D333">
+        <v>4</v>
+      </c>
+      <c r="E333">
+        <v>3</v>
+      </c>
+      <c r="F333" t="s">
+        <v>18</v>
+      </c>
+      <c r="G333" t="s">
+        <v>34</v>
+      </c>
       <c r="H333" s="8"/>
       <c r="I333">
         <f t="shared" si="16"/>
@@ -25516,7 +25722,7 @@
       </c>
       <c r="J333">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K333">
         <f t="shared" si="16"/>
@@ -25532,11 +25738,32 @@
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B334" s="7"/>
+      <c r="A334" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="B334" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C334" t="s">
+        <v>28</v>
+      </c>
+      <c r="D334">
+        <f>98-34</f>
+        <v>64</v>
+      </c>
+      <c r="E334">
+        <v>1.2</v>
+      </c>
+      <c r="F334" t="s">
+        <v>18</v>
+      </c>
+      <c r="G334" t="s">
+        <v>15</v>
+      </c>
       <c r="H334" s="8"/>
       <c r="I334">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>76.8</v>
       </c>
       <c r="J334">
         <f t="shared" si="16"/>
@@ -25556,11 +25783,31 @@
       </c>
     </row>
     <row r="335" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B335" s="7"/>
+      <c r="A335" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B335" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C335" t="s">
+        <v>27</v>
+      </c>
+      <c r="D335">
+        <v>1</v>
+      </c>
+      <c r="E335">
+        <v>1</v>
+      </c>
+      <c r="F335" t="s">
+        <v>18</v>
+      </c>
+      <c r="G335" t="s">
+        <v>15</v>
+      </c>
       <c r="H335" s="8"/>
       <c r="I335">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J335">
         <f t="shared" si="16"/>
@@ -25580,7 +25827,28 @@
       </c>
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B336" s="7"/>
+      <c r="A336" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B336" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C336" t="s">
+        <v>28</v>
+      </c>
+      <c r="D336">
+        <f>14+14+14+14</f>
+        <v>56</v>
+      </c>
+      <c r="E336">
+        <v>3</v>
+      </c>
+      <c r="F336" t="s">
+        <v>18</v>
+      </c>
+      <c r="G336" t="s">
+        <v>234</v>
+      </c>
       <c r="H336" s="8"/>
       <c r="I336">
         <f t="shared" si="16"/>
@@ -25600,11 +25868,31 @@
       </c>
       <c r="M336" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B337" s="7"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A337" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B337" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C337" t="s">
+        <v>149</v>
+      </c>
+      <c r="D337">
+        <v>17</v>
+      </c>
+      <c r="E337">
+        <v>1.3</v>
+      </c>
+      <c r="F337" t="s">
+        <v>18</v>
+      </c>
+      <c r="G337" t="s">
+        <v>88</v>
+      </c>
       <c r="H337" s="8"/>
       <c r="I337">
         <f t="shared" si="16"/>
@@ -25616,7 +25904,7 @@
       </c>
       <c r="K337">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>22.1</v>
       </c>
       <c r="L337">
         <f t="shared" si="16"/>
@@ -25627,8 +25915,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B338" s="7"/>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A338" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B338" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C338" t="s">
+        <v>149</v>
+      </c>
+      <c r="D338">
+        <v>4</v>
+      </c>
+      <c r="E338">
+        <v>3</v>
+      </c>
+      <c r="F338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338" t="s">
+        <v>234</v>
+      </c>
       <c r="H338" s="8"/>
       <c r="I338">
         <f t="shared" si="16"/>
@@ -25648,11 +25956,31 @@
       </c>
       <c r="M338" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B339" s="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A339" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B339" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C339" t="s">
+        <v>149</v>
+      </c>
+      <c r="D339">
+        <v>29</v>
+      </c>
+      <c r="E339">
+        <v>1</v>
+      </c>
+      <c r="F339" t="s">
+        <v>18</v>
+      </c>
+      <c r="G339" t="s">
+        <v>88</v>
+      </c>
       <c r="H339" s="8"/>
       <c r="I339">
         <f t="shared" si="16"/>
@@ -25664,7 +25992,7 @@
       </c>
       <c r="K339">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L339">
         <f t="shared" si="16"/>
@@ -25675,8 +26003,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B340" s="7"/>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A340" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="B340" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C340" t="s">
+        <v>149</v>
+      </c>
+      <c r="D340">
+        <v>46</v>
+      </c>
+      <c r="E340">
+        <v>2</v>
+      </c>
+      <c r="F340" t="s">
+        <v>18</v>
+      </c>
+      <c r="G340" t="s">
+        <v>88</v>
+      </c>
       <c r="H340" s="8"/>
       <c r="I340">
         <f t="shared" si="16"/>
@@ -25688,7 +26036,7 @@
       </c>
       <c r="K340">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="L340">
         <f t="shared" si="16"/>
@@ -25699,8 +26047,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B341" s="7"/>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>128</v>
+      </c>
+      <c r="B341" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C341" t="s">
+        <v>149</v>
+      </c>
+      <c r="D341">
+        <v>6</v>
+      </c>
+      <c r="E341">
+        <v>1</v>
+      </c>
+      <c r="F341" t="s">
+        <v>18</v>
+      </c>
+      <c r="G341" t="s">
+        <v>88</v>
+      </c>
       <c r="H341" s="8"/>
       <c r="I341">
         <f t="shared" si="16"/>
@@ -25712,7 +26080,7 @@
       </c>
       <c r="K341">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L341">
         <f t="shared" si="16"/>
@@ -25723,8 +26091,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B342" s="7"/>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A342" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="B342" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C342" t="s">
+        <v>173</v>
+      </c>
+      <c r="D342">
+        <v>-46</v>
+      </c>
+      <c r="E342">
+        <v>0</v>
+      </c>
+      <c r="F342" t="s">
+        <v>18</v>
+      </c>
+      <c r="G342" t="s">
+        <v>88</v>
+      </c>
       <c r="H342" s="8"/>
       <c r="I342">
         <f t="shared" si="16"/>
@@ -25747,12 +26135,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B343" s="7"/>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A343" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B343" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C343" t="s">
+        <v>149</v>
+      </c>
+      <c r="D343">
+        <v>1</v>
+      </c>
+      <c r="E343">
+        <v>1</v>
+      </c>
+      <c r="F343" t="s">
+        <v>18</v>
+      </c>
+      <c r="G343" t="s">
+        <v>15</v>
+      </c>
       <c r="H343" s="8"/>
       <c r="I343">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J343">
         <f t="shared" si="16"/>
@@ -25771,12 +26179,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B344" s="7"/>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A344" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B344" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C344" t="s">
+        <v>149</v>
+      </c>
+      <c r="D344">
+        <f>12+4</f>
+        <v>16</v>
+      </c>
+      <c r="E344">
+        <v>1.2</v>
+      </c>
+      <c r="F344" t="s">
+        <v>18</v>
+      </c>
+      <c r="G344" t="s">
+        <v>15</v>
+      </c>
       <c r="H344" s="8"/>
       <c r="I344">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="J344">
         <f t="shared" si="16"/>
@@ -25795,8 +26224,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B345" s="7"/>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A345" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="B345" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C345" t="s">
+        <v>149</v>
+      </c>
+      <c r="D345">
+        <v>10</v>
+      </c>
+      <c r="E345">
+        <v>1</v>
+      </c>
+      <c r="F345" t="s">
+        <v>18</v>
+      </c>
+      <c r="G345" t="s">
+        <v>34</v>
+      </c>
       <c r="H345" s="8"/>
       <c r="I345">
         <f t="shared" si="16"/>
@@ -25804,7 +26253,7 @@
       </c>
       <c r="J345">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K345">
         <f t="shared" si="16"/>
@@ -25819,8 +26268,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B346" s="7"/>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A346" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B346" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C346" t="s">
+        <v>149</v>
+      </c>
+      <c r="D346">
+        <f>37+144+43</f>
+        <v>224</v>
+      </c>
+      <c r="E346">
+        <v>2</v>
+      </c>
+      <c r="F346" t="s">
+        <v>18</v>
+      </c>
+      <c r="G346" t="s">
+        <v>34</v>
+      </c>
       <c r="H346" s="8"/>
       <c r="I346">
         <f t="shared" si="16"/>
@@ -25828,7 +26298,7 @@
       </c>
       <c r="J346">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="K346">
         <f t="shared" si="16"/>
@@ -25843,8 +26313,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B347" s="7"/>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>214</v>
+      </c>
+      <c r="B347" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C347" t="s">
+        <v>27</v>
+      </c>
+      <c r="D347">
+        <v>1</v>
+      </c>
+      <c r="E347">
+        <v>3</v>
+      </c>
+      <c r="F347" t="s">
+        <v>18</v>
+      </c>
+      <c r="G347" t="s">
+        <v>34</v>
+      </c>
       <c r="H347" s="8"/>
       <c r="I347">
         <f t="shared" si="16"/>
@@ -25852,7 +26342,7 @@
       </c>
       <c r="J347">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K347">
         <f t="shared" si="16"/>
@@ -25867,8 +26357,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B348" s="7"/>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>214</v>
+      </c>
+      <c r="B348" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C348" t="s">
+        <v>149</v>
+      </c>
+      <c r="D348">
+        <v>2</v>
+      </c>
+      <c r="E348">
+        <v>3</v>
+      </c>
+      <c r="F348" t="s">
+        <v>18</v>
+      </c>
+      <c r="G348" t="s">
+        <v>34</v>
+      </c>
       <c r="H348" s="8"/>
       <c r="I348">
         <f t="shared" si="16"/>
@@ -25876,7 +26386,7 @@
       </c>
       <c r="J348">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K348">
         <f t="shared" si="16"/>
@@ -25891,8 +26401,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B349" s="7"/>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>214</v>
+      </c>
+      <c r="B349" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C349" t="s">
+        <v>149</v>
+      </c>
+      <c r="D349">
+        <v>3</v>
+      </c>
+      <c r="E349">
+        <v>3</v>
+      </c>
+      <c r="F349" t="s">
+        <v>18</v>
+      </c>
+      <c r="G349" t="s">
+        <v>34</v>
+      </c>
       <c r="H349" s="8"/>
       <c r="I349">
         <f t="shared" si="16"/>
@@ -25900,7 +26430,7 @@
       </c>
       <c r="J349">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K349">
         <f t="shared" si="16"/>
@@ -25915,8 +26445,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B350" s="7"/>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>214</v>
+      </c>
+      <c r="B350" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C350" t="s">
+        <v>149</v>
+      </c>
+      <c r="D350">
+        <v>1</v>
+      </c>
+      <c r="E350">
+        <v>3</v>
+      </c>
+      <c r="F350" t="s">
+        <v>18</v>
+      </c>
+      <c r="G350" t="s">
+        <v>34</v>
+      </c>
       <c r="H350" s="8"/>
       <c r="I350">
         <f t="shared" si="16"/>
@@ -25924,7 +26474,7 @@
       </c>
       <c r="J350">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K350">
         <f t="shared" si="16"/>
@@ -25939,12 +26489,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B351" s="7"/>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A351" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B351" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C351" t="s">
+        <v>27</v>
+      </c>
+      <c r="D351">
+        <v>8</v>
+      </c>
+      <c r="E351">
+        <v>1</v>
+      </c>
+      <c r="F351" t="s">
+        <v>18</v>
+      </c>
+      <c r="G351" t="s">
+        <v>15</v>
+      </c>
       <c r="H351" s="8"/>
       <c r="I351">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J351">
         <f t="shared" si="16"/>
@@ -25963,12 +26533,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B352" s="7"/>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>128</v>
+      </c>
+      <c r="B352" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C352" t="s">
+        <v>27</v>
+      </c>
+      <c r="D352">
+        <f>2+4+23+13+13</f>
+        <v>55</v>
+      </c>
+      <c r="E352">
+        <v>0.8</v>
+      </c>
+      <c r="F352" t="s">
+        <v>18</v>
+      </c>
+      <c r="G352" t="s">
+        <v>15</v>
+      </c>
       <c r="H352" s="8"/>
       <c r="I352">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="J352">
         <f t="shared" si="16"/>
@@ -25987,8 +26578,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B353" s="7"/>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A353" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="B353" s="7" t="s">
+        <v>264</v>
+      </c>
       <c r="H353" s="8"/>
       <c r="I353">
         <f t="shared" ref="I353:M403" si="17">MAX(0, IF($G353=I$2, $D353*$E353, 0))</f>
@@ -26011,7 +26607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B354" s="7"/>
       <c r="H354" s="8"/>
       <c r="I354">
@@ -26035,7 +26631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B355" s="7"/>
       <c r="H355" s="8"/>
       <c r="I355">
@@ -26059,7 +26655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B356" s="7"/>
       <c r="H356" s="8"/>
       <c r="I356">
@@ -26083,7 +26679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B357" s="7"/>
       <c r="H357" s="8"/>
       <c r="I357">
@@ -26107,7 +26703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B358" s="7"/>
       <c r="H358" s="8"/>
       <c r="I358">
@@ -26131,7 +26727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B359" s="7"/>
       <c r="H359" s="8"/>
       <c r="I359">
@@ -26155,7 +26751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B360" s="7"/>
       <c r="H360" s="8"/>
       <c r="I360">
@@ -26179,7 +26775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B361" s="7"/>
       <c r="H361" s="8"/>
       <c r="I361">
@@ -26203,7 +26799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B362" s="7"/>
       <c r="H362" s="8"/>
       <c r="I362">
@@ -26227,7 +26823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B363" s="7"/>
       <c r="H363" s="8"/>
       <c r="I363">
@@ -26251,7 +26847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B364" s="7"/>
       <c r="H364" s="8"/>
       <c r="I364">
@@ -26275,7 +26871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B365" s="7"/>
       <c r="H365" s="8"/>
       <c r="I365">
@@ -26299,7 +26895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B366" s="7"/>
       <c r="H366" s="8"/>
       <c r="I366">
@@ -26323,7 +26919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B367" s="7"/>
       <c r="H367" s="8"/>
       <c r="I367">
@@ -26347,7 +26943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B368" s="7"/>
       <c r="H368" s="8"/>
       <c r="I368">
@@ -29566,15 +30162,15 @@
       </c>
       <c r="I501" s="10">
         <f>SUM(I$3:INDEX(I:I,$F$1))</f>
-        <v>4695.7999999999993</v>
+        <v>4890.7999999999993</v>
       </c>
       <c r="J501" s="10">
         <f>SUM(J$3:INDEX(J:J,$F$1))</f>
-        <v>4702.3</v>
+        <v>5281.9000000000005</v>
       </c>
       <c r="K501" s="10">
         <f>SUM(K$3:INDEX(K:K,$F$1))</f>
-        <v>1403</v>
+        <v>1552.1</v>
       </c>
       <c r="L501" s="10">
         <f>SUM(L$3:INDEX(L:L,$F$1))</f>
@@ -29582,7 +30178,7 @@
       </c>
       <c r="M501" s="10">
         <f>SUM(M$3:INDEX(M:M,$F$1))</f>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="502" spans="1:13" x14ac:dyDescent="0.25">
@@ -29594,19 +30190,19 @@
       </c>
       <c r="I502" cm="1">
         <f t="array" ref="I502">SUM(_xlfn._xlws.FILTER(I$3:INDEX(I:I,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(I$3:INDEX(I:I,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(I$3:INDEX(I:I,$F$1))), MIN($H$502, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
-        <v>127.2</v>
+        <v>72.2</v>
       </c>
       <c r="J502" cm="1">
         <f t="array" ref="J502">SUM(_xlfn._xlws.FILTER(J$3:INDEX(J:J,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(J$3:INDEX(J:J,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(J$3:INDEX(J:J,$F$1))), MIN($H$502, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
-        <v>194</v>
+        <v>479</v>
       </c>
       <c r="K502" cm="1">
         <f t="array" ref="K502">SUM(_xlfn._xlws.FILTER(K$3:INDEX(K:K,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(K$3:INDEX(K:K,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(K$3:INDEX(K:K,$F$1))), MIN($H$502, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L502" cm="1">
         <f t="array" ref="L502">SUM(_xlfn._xlws.FILTER(L$3:INDEX(L:L,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(L$3:INDEX(L:L,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(L$3:INDEX(L:L,$F$1))), MIN($H$502, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="M502" cm="1">
         <f t="array" ref="M502">SUM(_xlfn._xlws.FILTER(M$3:INDEX(M:M,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (ROW(M$3:INDEX(M:M,$F$1)) &gt;= LARGE(IF($G$3:INDEX($G:$G,$F$1)&lt;&gt;"", ROW(M$3:INDEX(M:M,$F$1))), MIN($H$502, COUNTIF($G$3:INDEX($G:$G,$F$1), "&lt;&gt;"))))))</f>
@@ -29622,15 +30218,15 @@
       </c>
       <c r="I503" cm="1">
         <f t="array" ref="I503">IFERROR(SUM(_xlfn._xlws.FILTER(I$3:INDEX(I:I,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (I$3:INDEX(I:I,$F$1) &gt; 0) * (ROW(I$3:INDEX(I:I,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (I$3:INDEX(I:I,$F$1) &gt; 0), ROW(I$3:INDEX(I:I,$F$1))), MIN($H$503, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", I$3:INDEX(I:I,$F$1), "&gt;0")))))), 0)</f>
-        <v>316</v>
+        <v>430.2</v>
       </c>
       <c r="J503" cm="1">
         <f t="array" ref="J503">IFERROR(SUM(_xlfn._xlws.FILTER(J$3:INDEX(J:J,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (J$3:INDEX(J:J,$F$1) &gt; 0) * (ROW(J$3:INDEX(J:J,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (J$3:INDEX(J:J,$F$1) &gt; 0), ROW(J$3:INDEX(J:J,$F$1))), MIN($H$503, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", J$3:INDEX(J:J,$F$1), "&gt;0")))))), 0)</f>
-        <v>680</v>
+        <v>808.8</v>
       </c>
       <c r="K503" cm="1">
         <f t="array" ref="K503">IFERROR(SUM(_xlfn._xlws.FILTER(K$3:INDEX(K:K,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (K$3:INDEX(K:K,$F$1) &gt; 0) * (ROW(K$3:INDEX(K:K,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (K$3:INDEX(K:K,$F$1) &gt; 0), ROW(K$3:INDEX(K:K,$F$1))), MIN($H$503, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", K$3:INDEX(K:K,$F$1), "&gt;0")))))), 0)</f>
-        <v>982</v>
+        <v>794.1</v>
       </c>
       <c r="L503" cm="1">
         <f t="array" ref="L503">IFERROR(SUM(_xlfn._xlws.FILTER(L$3:INDEX(L:L,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (L$3:INDEX(L:L,$F$1) &gt; 0) * (ROW(L$3:INDEX(L:L,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (L$3:INDEX(L:L,$F$1) &gt; 0), ROW(L$3:INDEX(L:L,$F$1))), MIN($H$503, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", L$3:INDEX(L:L,$F$1), "&gt;0")))))), 0)</f>
@@ -29638,7 +30234,7 @@
       </c>
       <c r="M503" cm="1">
         <f t="array" ref="M503">IFERROR(SUM(_xlfn._xlws.FILTER(M$3:INDEX(M:M,$F$1), ($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (M$3:INDEX(M:M,$F$1) &gt; 0) * (ROW(M$3:INDEX(M:M,$F$1)) &gt;= LARGE(IF(($G$3:INDEX($G:$G,$F$1)&lt;&gt;"") * (M$3:INDEX(M:M,$F$1) &gt; 0), ROW(M$3:INDEX(M:M,$F$1))), MIN($H$503, COUNTIFS($G$3:INDEX($G:$G,$F$1), "&lt;&gt;", M$3:INDEX(M:M,$F$1), "&gt;0")))))), 0)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="504" spans="1:13" x14ac:dyDescent="0.25">
@@ -29669,15 +30265,15 @@
       </c>
       <c r="I505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), I$2)</f>
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="J505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), J$2)</f>
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="K505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), K$2)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), L$2)</f>
@@ -29685,7 +30281,7 @@
       </c>
       <c r="M505">
         <f>COUNTIF($G$3:INDEX($G:$G,$F$1), M$2)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="506" spans="1:13" x14ac:dyDescent="0.25">
@@ -29694,15 +30290,15 @@
       </c>
       <c r="I506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
-        <v>1.2495412844036695</v>
+        <v>1.2427350427350425</v>
       </c>
       <c r="J506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
-        <v>1.3524137931034481</v>
+        <v>1.399354838709677</v>
       </c>
       <c r="K506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), K$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), K$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
-        <v>1.5</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="L506">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), L$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), L$2, $E$3:INDEX($E:$E,$F$1)), 0)</f>
@@ -29719,15 +30315,15 @@
       </c>
       <c r="I507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), I$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), I$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
-        <v>28.311926605504588</v>
+        <v>27.743589743589745</v>
       </c>
       <c r="J507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), J$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), J$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
-        <v>19.627586206896552</v>
+        <v>20.677419354838708</v>
       </c>
       <c r="K507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), K$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), K$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
-        <v>32.85</v>
+        <v>28.36</v>
       </c>
       <c r="L507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), L$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), L$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
@@ -29735,7 +30331,7 @@
       </c>
       <c r="M507">
         <f>IF(COUNTIF($G$3:INDEX($G:$G,$F$1), M$2) &gt; 0, AVERAGEIF($G$3:INDEX($G:$G,$F$1), M$2, $D$3:INDEX($D:$D,$F$1)), 0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="508" spans="1:13" x14ac:dyDescent="0.25">
@@ -29744,15 +30340,15 @@
       </c>
       <c r="I508">
         <f>ROUND(I$505*I$506*I$507, 0)</f>
-        <v>3856</v>
+        <v>4034</v>
       </c>
       <c r="J508">
         <f>ROUND(J$505*J$506*J$507, 0)</f>
-        <v>3876</v>
+        <v>4514</v>
       </c>
       <c r="K508">
         <f>ROUND(K$505*K$506*K$507, 0)</f>
-        <v>986</v>
+        <v>1001</v>
       </c>
       <c r="L508">
         <f>ROUND(L$505*L$506*L$507, 0)</f>
@@ -29795,11 +30391,11 @@
       </c>
       <c r="I511">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$510, $C$3:INDEX($C:$C,$F$1), $G511)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J511">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$510, $C$3:INDEX($C:$C,$F$1), $G511)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K511">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$510, $C$3:INDEX($C:$C,$F$1), $G511)</f>
@@ -29811,7 +30407,7 @@
       </c>
       <c r="M511">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$510, $C$3:INDEX($C:$C,$F$1), $G511)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:13" x14ac:dyDescent="0.25">
@@ -29820,11 +30416,11 @@
       </c>
       <c r="I512">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$510, $C$3:INDEX($C:$C,$F$1), $G512)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J512">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$510, $C$3:INDEX($C:$C,$F$1), $G512)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K512">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$510, $C$3:INDEX($C:$C,$F$1), $G512)</f>
@@ -29928,7 +30524,7 @@
       </c>
       <c r="K516">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$510, $C$3:INDEX($C:$C,$F$1), $G516)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L516">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$510, $C$3:INDEX($C:$C,$F$1), $G516)</f>
@@ -29995,15 +30591,15 @@
       </c>
       <c r="I519">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$510, $C$3:INDEX($C:$C,$F$1), $G519)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J519">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$510, $C$3:INDEX($C:$C,$F$1), $G519)</f>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K519">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$510, $C$3:INDEX($C:$C,$F$1), $G519)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L519">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$510, $C$3:INDEX($C:$C,$F$1), $G519)</f>
@@ -30011,7 +30607,7 @@
       </c>
       <c r="M519">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$510, $C$3:INDEX($C:$C,$F$1), $G519)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="520" spans="7:13" x14ac:dyDescent="0.25">
@@ -30126,15 +30722,15 @@
       </c>
       <c r="I526">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), I$525, $F$3:INDEX($F:$F,$F$1), $G526)</f>
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="J526">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$525, $F$3:INDEX($F:$F,$F$1), $G526)</f>
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K526">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$525, $F$3:INDEX($F:$F,$F$1), $G526)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L526">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), L$525, $F$3:INDEX($F:$F,$F$1), $G526)</f>
@@ -30142,7 +30738,7 @@
       </c>
       <c r="M526">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), M$525, $F$3:INDEX($F:$F,$F$1), $G526)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="527" spans="7:13" x14ac:dyDescent="0.25">
@@ -30180,7 +30776,7 @@
       </c>
       <c r="J528">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), J$525, $F$3:INDEX($F:$F,$F$1), $G528)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K528">
         <f>COUNTIFS($G$3:INDEX($G:$G,$F$1), K$525, $F$3:INDEX($F:$F,$F$1), $G528)</f>
@@ -30323,27 +30919,27 @@
       </c>
       <c r="H536">
         <f>SUM(I501:M501)</f>
-        <v>14593.599999999999</v>
+        <v>15697.300000000001</v>
       </c>
       <c r="I536" s="16">
         <f>I501/$H536</f>
-        <v>0.32177118736980592</v>
+        <v>0.31156950558376273</v>
       </c>
       <c r="J536" s="16">
         <f>J501/$H536</f>
-        <v>0.32221658809341086</v>
+        <v>0.33648461837386051</v>
       </c>
       <c r="K536" s="16">
         <f>K501/$H536</f>
-        <v>9.6138033110404572E-2</v>
+        <v>9.8876876915138259E-2</v>
       </c>
       <c r="L536" s="16">
         <f>L501/$H536</f>
-        <v>0.25987419142637869</v>
+        <v>0.24160205895281353</v>
       </c>
       <c r="M536" s="16">
         <f>M501/$H536</f>
-        <v>0</v>
+        <v>1.14669401744249E-2</v>
       </c>
     </row>
   </sheetData>
@@ -30498,10 +31094,26 @@
     <hyperlink ref="A324" r:id="rId145" xr:uid="{69E6B5BE-C75F-4DCF-9F04-DE748577573F}"/>
     <hyperlink ref="A326" r:id="rId146" xr:uid="{767A3ED2-94F0-472F-BAC7-6AD204629CC8}"/>
     <hyperlink ref="A327" r:id="rId147" xr:uid="{89D0DE87-BFB9-4160-8911-7E9A1AE7C1D9}"/>
+    <hyperlink ref="A328" r:id="rId148" xr:uid="{636DBEDB-76AA-4972-AFCF-37DB4193EC9A}"/>
+    <hyperlink ref="A331" r:id="rId149" xr:uid="{3ECBCF44-C7D8-4FB2-9FDB-DAF155D43BC9}"/>
+    <hyperlink ref="A334" r:id="rId150" xr:uid="{6985873E-8A2B-4BDB-8EE1-D919F32ADE56}"/>
+    <hyperlink ref="A335" r:id="rId151" xr:uid="{02B69DEC-E1F3-4667-A56B-846867EB15CA}"/>
+    <hyperlink ref="A336" r:id="rId152" xr:uid="{27E54B8E-1900-4122-A0A4-B9170A7FF377}"/>
+    <hyperlink ref="A337" r:id="rId153" xr:uid="{F4A7C2AA-F710-46EB-8972-758C43FDD8B2}"/>
+    <hyperlink ref="A338" r:id="rId154" xr:uid="{E966BDB0-8DB2-4A57-BDEF-734F8FF0E5C7}"/>
+    <hyperlink ref="A339" r:id="rId155" xr:uid="{3D1DD4BB-770E-489F-8784-33E28197B761}"/>
+    <hyperlink ref="A340" r:id="rId156" xr:uid="{81F94012-CE14-4E63-B1EA-B93A919402B9}"/>
+    <hyperlink ref="A342" r:id="rId157" xr:uid="{7AD31F94-3AFE-4638-BC90-C775617F2528}"/>
+    <hyperlink ref="A343" r:id="rId158" xr:uid="{CA4CEA90-234D-4D0A-A924-8796BABFB082}"/>
+    <hyperlink ref="A344" r:id="rId159" xr:uid="{A88D1062-F42E-441C-AEA8-163FE9B4D2E5}"/>
+    <hyperlink ref="A345" r:id="rId160" xr:uid="{FE20E249-10BA-4368-9233-363FF2E9F5AE}"/>
+    <hyperlink ref="A346" r:id="rId161" xr:uid="{E4C416C4-1C25-489C-930C-1B7037FF4355}"/>
+    <hyperlink ref="A351" r:id="rId162" xr:uid="{A722881F-02F5-41DB-96C8-0A54EDB0517E}"/>
+    <hyperlink ref="A353" r:id="rId163" xr:uid="{453ED6EC-FC5E-478D-A5D1-5CBBFF2F77CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId148"/>
-  <drawing r:id="rId149"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId164"/>
+  <drawing r:id="rId165"/>
 </worksheet>
 </file>
 
@@ -30513,7 +31125,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>